<commit_message>
Nov 16th upload v2
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -1725,10 +1725,10 @@
     <t>AGSKL Training</t>
   </si>
   <si>
-    <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\02 AGS TRAINING\20211130 UNCONCIOUS BIAS</t>
-  </si>
-  <si>
     <t>Training folder</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\02 AGS TRAINING</t>
   </si>
 </sst>
 </file>
@@ -2389,8 +2389,8 @@
   <dimension ref="A1:H9992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A241" sqref="A241"/>
+      <pane ySplit="8" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -5857,7 +5857,7 @@
         <v>470</v>
       </c>
       <c r="B240" s="12" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>123</v>
@@ -5868,10 +5868,10 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B241" s="12" t="s">
         <v>472</v>
-      </c>
-      <c r="B241" s="12" t="s">
-        <v>471</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Dec 20th Commit v2
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB6A38E-D5A3-4820-BB26-9263038585DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89371170-F008-427B-BC92-61FAA7345CE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="855">
   <si>
     <t>Kota</t>
     <phoneticPr fontId="1"/>
@@ -2886,6 +2886,9 @@
   </si>
   <si>
     <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\92 APPLICATION ACCESS\15 COGNOS</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
@@ -3549,8 +3552,8 @@
   <dimension ref="A1:H9989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A481" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="8" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B486" sqref="B486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -9734,6 +9737,9 @@
     <row r="434" spans="1:4">
       <c r="A434" s="1" t="s">
         <v>767</v>
+      </c>
+      <c r="B434" s="2" t="s">
+        <v>854</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Commit Dec 21 v1
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89371170-F008-427B-BC92-61FAA7345CE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9609D2-BF7D-456B-8431-997CA1E523FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="SOP" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$D$485</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$D$486</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="858">
   <si>
     <t>Kota</t>
     <phoneticPr fontId="1"/>
@@ -2889,6 +2889,15 @@
   </si>
   <si>
     <t>xxx</t>
+  </si>
+  <si>
+    <t>KPI Tableau</t>
+  </si>
+  <si>
+    <t>https://tableau.bi.alconcloud.com/#/site/FRAGlobal/workbooks/8033/views</t>
+  </si>
+  <si>
+    <t>FRA KPI Tableau</t>
   </si>
 </sst>
 </file>
@@ -3552,8 +3561,8 @@
   <dimension ref="A1:H9989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B486" sqref="B486"/>
+      <pane ySplit="8" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A489" sqref="A489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3613,7 +3622,7 @@
       </c>
       <c r="H2" s="29">
         <f>SUM(G2:G8)</f>
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1">
@@ -3744,7 +3753,7 @@
       </c>
       <c r="G8" s="10">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H8" s="29"/>
     </row>
@@ -10477,12 +10486,32 @@
       </c>
     </row>
     <row r="487" spans="1:4">
-      <c r="A487" s="1"/>
-      <c r="D487" s="1"/>
+      <c r="A487" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B487" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="C487" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D487" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="488" spans="1:4">
-      <c r="A488" s="1"/>
-      <c r="D488" s="1"/>
+      <c r="A488" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B488" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="C488" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D488" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="489" spans="1:4">
       <c r="A489" s="1"/>
@@ -48489,7 +48518,7 @@
       <c r="D9989" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D485" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D486" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="H2:H8"/>
   </mergeCells>
@@ -48854,12 +48883,14 @@
     <hyperlink ref="B484" r:id="rId322" xr:uid="{27069D77-595B-4575-8191-029ECA0CBEDF}"/>
     <hyperlink ref="B485" r:id="rId323" xr:uid="{7FE4B831-BB1D-4394-8630-3D90EC986C07}"/>
     <hyperlink ref="B486" r:id="rId324" xr:uid="{EC076AE4-F7A3-4C5F-9490-856CE13CA761}"/>
+    <hyperlink ref="B487" r:id="rId325" location="/site/FRAGlobal/workbooks/8033/views" xr:uid="{45D05C47-B66F-4AFE-8400-89C4B056679A}"/>
+    <hyperlink ref="B488" r:id="rId326" location="/site/FRAGlobal/workbooks/8033/views" xr:uid="{05342276-7BF8-446A-8757-ACF9F57C52AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId325"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId327"/>
   <customProperties>
-    <customPr name="_pios_id" r:id="rId326"/>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId327"/>
+    <customPr name="_pios_id" r:id="rId328"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId329"/>
   </customProperties>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>

<commit_message>
Commit Jan 5th v2
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC2DB74-4B45-4CB6-B2AE-00BDBE2E6CE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD3F5B5-1E7D-4689-9D71-AD63AAA3E2FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3071,13 +3071,13 @@
     <t>Appzen Configuration Management Process</t>
   </si>
   <si>
-    <t>&lt;a href = "\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\07 T&amp;E OPERATIONAL GOVERNANCE\20210512 7_TE Operational Governance_12 May..pptx"&gt;Management Process&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Seat and Group</t>
   </si>
   <si>
-    <t>&lt;a href = ""\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\Team &amp; Workstation No.xlsx""&gt;Management Process&lt;/a&gt;</t>
+    <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\Team &amp; Workstation No.xlsx</t>
+  </si>
+  <si>
+    <t>"\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\07 T&amp;E OPERATIONAL GOVERNANCE\20210512 7_TE Operational Governance_12 May..pptx</t>
   </si>
 </sst>
 </file>
@@ -11160,7 +11160,7 @@
         <v>909</v>
       </c>
       <c r="B521" s="12" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C521" s="2" t="s">
         <v>32</v>
@@ -11171,10 +11171,10 @@
     </row>
     <row r="522" spans="1:4">
       <c r="A522" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="B522" s="12" t="s">
         <v>911</v>
-      </c>
-      <c r="B522" s="12" t="s">
-        <v>912</v>
       </c>
       <c r="C522" s="2" t="s">
         <v>123</v>
@@ -49459,7 +49459,7 @@
     <hyperlink ref="B506" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
     <hyperlink ref="B519" r:id="rId337" xr:uid="{F720CA53-E902-4015-99E7-CF7ED36AC79D}"/>
     <hyperlink ref="B521" r:id="rId338" display="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\07 T&amp;E OPERATIONAL GOVERNANCE\20210512 7_TE Operational Governance_12 May..pptx" xr:uid="{3CCDE37B-D158-43AD-A978-3B78F9D9BA39}"/>
-    <hyperlink ref="B522" r:id="rId339" display="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\07 T&amp;E OPERATIONAL GOVERNANCE\20210512 7_TE Operational Governance_12 May..pptx" xr:uid="{ADF26670-EF5D-48BD-A644-A0CF8811E942}"/>
+    <hyperlink ref="B522" r:id="rId339" xr:uid="{ADF26670-EF5D-48BD-A644-A0CF8811E942}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId340"/>

</xml_diff>

<commit_message>
Commit Jan 5th v3
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD3F5B5-1E7D-4689-9D71-AD63AAA3E2FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B105ECE0-BDF9-490D-8788-7E95F2120C97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="914">
   <si>
     <t>Kota</t>
     <phoneticPr fontId="1"/>
@@ -3077,7 +3077,10 @@
     <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\Team &amp; Workstation No.xlsx</t>
   </si>
   <si>
-    <t>"\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\07 T&amp;E OPERATIONAL GOVERNANCE\20210512 7_TE Operational Governance_12 May..pptx</t>
+    <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\07 T&amp;E OPERATIONAL GOVERNANCE\20210512 7_TE Operational Governance_12 May..pptx</t>
+  </si>
+  <si>
+    <t>Group and Seat</t>
   </si>
 </sst>
 </file>
@@ -3741,8 +3744,8 @@
   <dimension ref="A1:H9989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B522" sqref="B522"/>
+      <pane ySplit="8" topLeftCell="A512" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A523" sqref="A523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3802,7 +3805,7 @@
       </c>
       <c r="H2" s="29">
         <f>SUM(G2:G8)</f>
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1">
@@ -3933,7 +3936,7 @@
       </c>
       <c r="G8" s="10">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H8" s="29"/>
     </row>
@@ -11184,8 +11187,18 @@
       </c>
     </row>
     <row r="523" spans="1:4">
-      <c r="A523" s="1"/>
-      <c r="D523" s="1"/>
+      <c r="A523" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B523" s="12" t="s">
+        <v>911</v>
+      </c>
+      <c r="C523" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D523" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="524" spans="1:4">
       <c r="A524" s="1"/>
@@ -49458,14 +49471,15 @@
     <hyperlink ref="B501" r:id="rId335" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
     <hyperlink ref="B506" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
     <hyperlink ref="B519" r:id="rId337" xr:uid="{F720CA53-E902-4015-99E7-CF7ED36AC79D}"/>
-    <hyperlink ref="B521" r:id="rId338" display="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\07 T&amp;E OPERATIONAL GOVERNANCE\20210512 7_TE Operational Governance_12 May..pptx" xr:uid="{3CCDE37B-D158-43AD-A978-3B78F9D9BA39}"/>
+    <hyperlink ref="B521" r:id="rId338" xr:uid="{3CCDE37B-D158-43AD-A978-3B78F9D9BA39}"/>
     <hyperlink ref="B522" r:id="rId339" xr:uid="{ADF26670-EF5D-48BD-A644-A0CF8811E942}"/>
+    <hyperlink ref="B523" r:id="rId340" xr:uid="{7555B120-F5B3-469E-A7E2-CA5642A357B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId340"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId341"/>
   <customProperties>
-    <customPr name="_pios_id" r:id="rId341"/>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId342"/>
+    <customPr name="_pios_id" r:id="rId342"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId343"/>
   </customProperties>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -49546,7 +49560,7 @@
           <x14:formula1>
             <xm:f>Category!$A$2:$A$25</xm:f>
           </x14:formula1>
-          <xm:sqref>C436:C1048576 C151:C158 C161:C171 C181:C336 C339:C431 C1:C144</xm:sqref>
+          <xm:sqref>C1:C144 C151:C158 C161:C171 C181:C336 C339:C431 C436:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Commit Jan 13th v1
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773B4035-513E-4924-AD6C-AC8ED14167CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -18,9 +17,9 @@
     <sheet name="SOP" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$D$494</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$D$549</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2301" uniqueCount="981">
   <si>
     <t>Kota</t>
     <phoneticPr fontId="1"/>
@@ -3082,9 +3081,6 @@
     <t>I:\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Hakimi\VOC</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>VOC meeting notes</t>
   </si>
   <si>
@@ -3092,12 +3088,213 @@
   </si>
   <si>
     <t>Finance Core Portal</t>
+  </si>
+  <si>
+    <t>FIKO table maintenance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\FIKO\20211011_APAC FIKO_EXT PERS_Other Tables Maitenance_V2 のコピー.xlsx</t>
+  </si>
+  <si>
+    <t>CLMD (Credit Limit)</t>
+  </si>
+  <si>
+    <t>DCNT (Debit / Credit note)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WOFF (Write offs) </t>
+  </si>
+  <si>
+    <t>Accrual Engine</t>
+  </si>
+  <si>
+    <t>/NVS/NFCM_USR_LT</t>
+  </si>
+  <si>
+    <t>/NVS/ACCR_USER  (table)</t>
+  </si>
+  <si>
+    <t>/NVS/ACCR_COCODE (table)</t>
+  </si>
+  <si>
+    <t>/N/NVS/ACCR_TAB_LOGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/N/NVS/ACCRUAL_ENGINE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIKO Limit exceptions </t>
+  </si>
+  <si>
+    <t>APUSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JENT (Journal Entry Workflow). </t>
+  </si>
+  <si>
+    <t>Thresholds for Journal Entries (JENT) Credit Limits (CLMD) AR Write offs (WOFF) Credit/Debit memo request workflows (DCNT)</t>
+  </si>
+  <si>
+    <t>Z8CFFIKO_LIM</t>
+  </si>
+  <si>
+    <t>/NVS/EXT_PERS</t>
+  </si>
+  <si>
+    <t>/NVS/APUSR</t>
+  </si>
+  <si>
+    <t>/NVS/NFCM_THRSLD</t>
+  </si>
+  <si>
+    <t>Hanis</t>
+  </si>
+  <si>
+    <t>Ain</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>Posted Reports Volume</t>
+  </si>
+  <si>
+    <t>"I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\02  T&amp;E\10  REPORT\AGS KL T&amp;E Exp Rpt Process 2020 2021.xlsx"</t>
+  </si>
+  <si>
+    <t>eTravel 2020</t>
+  </si>
+  <si>
+    <t>"I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\02  T&amp;E\10  REPORT\2020\etravel 2020.xlsx"</t>
+  </si>
+  <si>
+    <t>Direct Session List Name</t>
+  </si>
+  <si>
+    <t>"I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\02  T&amp;E\12 PROJECT\Direct Session List Name from Jan 2021.xlsx"</t>
+  </si>
+  <si>
+    <t>"I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\02  T&amp;E\12 PROJECT\1205 False Positive.xlsx"</t>
+  </si>
+  <si>
+    <t>False Positive</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\2  SOP\How to call Japanese numbers from Malaysia.docx</t>
+  </si>
+  <si>
+    <t>Purecloud call</t>
+  </si>
+  <si>
+    <t>Payment term</t>
+  </si>
+  <si>
+    <t>https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B897F2C36-6DBE-4A39-AD78-0CE171B4C537%7D&amp;file=Excel%E6%A4%9C%E7%B4%A2%E3%83%84%E3%83%BC%E3%83%AB.xlsm&amp;action=default&amp;mobileredirect=true</t>
+  </si>
+  <si>
+    <t>Identify payment term</t>
+  </si>
+  <si>
+    <t>You can search it via vendor list excel or via SAP T-code FK03</t>
+  </si>
+  <si>
+    <t>POT files</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\15 MONTHLY KPI\POT</t>
+  </si>
+  <si>
+    <t>VRT request manual</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\2  SOP\VMD_request_manual.docx</t>
+  </si>
+  <si>
+    <t>Team A</t>
+  </si>
+  <si>
+    <t>Team B</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File : team A</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File : team B</t>
+  </si>
+  <si>
+    <t>Purecloud</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File : How to call Japan vendor</t>
+  </si>
+  <si>
+    <t>Purecloud call vendor</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File : how to confirm invoice requestor</t>
+  </si>
+  <si>
+    <t>Invoice no PIC</t>
+  </si>
+  <si>
+    <t>Invoice PIC check</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
+  </si>
+  <si>
+    <t>Due Net Calculation</t>
+  </si>
+  <si>
+    <t>Invoice offset</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File : Kawami Shouri 56722537</t>
+  </si>
+  <si>
+    <t>Wrong Coding Offset</t>
+  </si>
+  <si>
+    <t>Late Payment Proposal</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File : late payment run</t>
+  </si>
+  <si>
+    <t>Late Proposal Iida</t>
+  </si>
+  <si>
+    <t>Malaysia Public Holiday</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File :Malaysia PH 2022</t>
+  </si>
+  <si>
+    <t>Refund fee</t>
+  </si>
+  <si>
+    <t>Henkin Tesuuryou</t>
+  </si>
+  <si>
+    <t>\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Syahmi
+File : 手数料</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -3456,7 +3653,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3751,12 +3948,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9989"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A515" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A525" sqref="A525"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="11" topLeftCell="C563" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="E563" sqref="E563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3773,7 +3972,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="13" t="s">
-        <v>914</v>
+        <v>947</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -3811,15 +4010,15 @@
         <v>25</v>
       </c>
       <c r="G2" s="10">
-        <f t="shared" ref="G2:G8" si="0">+COUNTIF($D:$D,F2)</f>
+        <f t="shared" ref="G2:G10" si="0">+COUNTIF($D:$D,F2)</f>
         <v>3</v>
       </c>
       <c r="H2" s="29">
         <f>SUM(G2:G8)</f>
-        <v>524</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="14.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>224</v>
       </c>
@@ -3837,7 +4036,7 @@
       </c>
       <c r="G3" s="10">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="H3" s="29"/>
     </row>
@@ -3881,7 +4080,7 @@
       </c>
       <c r="G5" s="10">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H5" s="29"/>
     </row>
@@ -3903,7 +4102,7 @@
       </c>
       <c r="G6" s="10">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="H6" s="29"/>
     </row>
@@ -3925,11 +4124,11 @@
       </c>
       <c r="G7" s="10">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="H7" s="29"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="14.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
@@ -3964,6 +4163,14 @@
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F9" s="11" t="s">
+        <v>936</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -3978,6 +4185,14 @@
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F10" s="11" t="s">
+        <v>937</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -11213,7 +11428,7 @@
     </row>
     <row r="524" spans="1:4">
       <c r="A524" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B524" s="2" t="s">
         <v>913</v>
@@ -11227,10 +11442,10 @@
     </row>
     <row r="525" spans="1:4">
       <c r="A525" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B525" s="12" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C525" s="2" t="s">
         <v>122</v>
@@ -11240,160 +11455,544 @@
       </c>
     </row>
     <row r="526" spans="1:4">
-      <c r="A526" s="1"/>
-      <c r="D526" s="1"/>
+      <c r="A526" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B526" s="12" t="s">
+        <v>918</v>
+      </c>
+      <c r="C526" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D526" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="527" spans="1:4">
-      <c r="A527" s="1"/>
-      <c r="D527" s="1"/>
+      <c r="A527" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B527" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="C527" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D527" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="528" spans="1:4">
-      <c r="A528" s="1"/>
-      <c r="D528" s="1"/>
+      <c r="A528" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B528" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="C528" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D528" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="529" spans="1:4">
-      <c r="A529" s="1"/>
-      <c r="D529" s="1"/>
+      <c r="A529" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B529" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="C529" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D529" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="530" spans="1:4">
-      <c r="A530" s="1"/>
-      <c r="D530" s="1"/>
+      <c r="A530" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="B530" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C530" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D530" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="531" spans="1:4">
-      <c r="A531" s="1"/>
-      <c r="D531" s="1"/>
+      <c r="A531" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="B531" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C531" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D531" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="532" spans="1:4">
-      <c r="A532" s="1"/>
-      <c r="D532" s="1"/>
+      <c r="A532" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B532" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C532" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="533" spans="1:4">
-      <c r="A533" s="1"/>
-      <c r="D533" s="1"/>
+      <c r="A533" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B533" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C533" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D533" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="534" spans="1:4">
-      <c r="A534" s="1"/>
-      <c r="D534" s="1"/>
+      <c r="A534" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B534" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C534" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D534" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="535" spans="1:4">
-      <c r="A535" s="1"/>
-      <c r="D535" s="1"/>
+      <c r="A535" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B535" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="C535" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D535" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="536" spans="1:4">
-      <c r="A536" s="1"/>
-      <c r="D536" s="1"/>
+      <c r="A536" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B536" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C536" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D536" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="537" spans="1:4">
-      <c r="A537" s="1"/>
-      <c r="D537" s="1"/>
+      <c r="A537" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B537" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="C537" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D537" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="538" spans="1:4">
-      <c r="A538" s="1"/>
-      <c r="D538" s="1"/>
+      <c r="A538" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B538" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="C538" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D538" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="539" spans="1:4">
-      <c r="A539" s="1"/>
-      <c r="D539" s="1"/>
+      <c r="A539" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B539" s="12" t="s">
+        <v>940</v>
+      </c>
+      <c r="C539" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D539" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="540" spans="1:4">
-      <c r="A540" s="1"/>
-      <c r="D540" s="1"/>
+      <c r="A540" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="B540" s="12" t="s">
+        <v>942</v>
+      </c>
+      <c r="C540" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D540" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="541" spans="1:4">
-      <c r="A541" s="1"/>
-      <c r="D541" s="1"/>
+      <c r="A541" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="B541" s="12" t="s">
+        <v>944</v>
+      </c>
+      <c r="C541" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D541" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="542" spans="1:4">
-      <c r="A542" s="1"/>
-      <c r="D542" s="1"/>
+      <c r="A542" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="B542" s="12" t="s">
+        <v>948</v>
+      </c>
+      <c r="C542" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D542" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="543" spans="1:4">
-      <c r="A543" s="1"/>
-      <c r="D543" s="1"/>
+      <c r="A543" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="B543" s="12" t="s">
+        <v>945</v>
+      </c>
+      <c r="C543" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D543" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="544" spans="1:4">
-      <c r="A544" s="1"/>
-      <c r="D544" s="1"/>
+      <c r="A544" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="B544" s="12" t="s">
+        <v>951</v>
+      </c>
+      <c r="C544" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D544" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="545" spans="1:4">
-      <c r="A545" s="1"/>
-      <c r="D545" s="1"/>
+      <c r="A545" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="C545" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D545" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="546" spans="1:4">
-      <c r="A546" s="1"/>
-      <c r="D546" s="1"/>
+      <c r="A546" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B546" s="12" t="s">
+        <v>955</v>
+      </c>
+      <c r="C546" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D546" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="547" spans="1:4">
-      <c r="A547" s="1"/>
-      <c r="D547" s="1"/>
-    </row>
-    <row r="548" spans="1:4">
-      <c r="A548" s="1"/>
-      <c r="D548" s="1"/>
+      <c r="A547" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B547" s="12" t="s">
+        <v>957</v>
+      </c>
+      <c r="C547" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D547" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4" ht="13" customHeight="1">
+      <c r="A548" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="B548" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="D548" s="1" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="549" spans="1:4">
-      <c r="A549" s="1"/>
-      <c r="D549" s="1"/>
-    </row>
-    <row r="550" spans="1:4">
-      <c r="A550" s="1"/>
-      <c r="D550" s="1"/>
-    </row>
-    <row r="551" spans="1:4">
-      <c r="A551" s="1"/>
-      <c r="D551" s="1"/>
-    </row>
-    <row r="552" spans="1:4">
-      <c r="A552" s="1"/>
-      <c r="D552" s="1"/>
-    </row>
-    <row r="553" spans="1:4">
-      <c r="A553" s="1"/>
-      <c r="D553" s="1"/>
-    </row>
-    <row r="554" spans="1:4">
-      <c r="A554" s="1"/>
-      <c r="D554" s="1"/>
-    </row>
-    <row r="555" spans="1:4">
-      <c r="A555" s="1"/>
-      <c r="D555" s="1"/>
-    </row>
-    <row r="556" spans="1:4">
-      <c r="A556" s="1"/>
-      <c r="D556" s="1"/>
-    </row>
-    <row r="557" spans="1:4">
-      <c r="A557" s="1"/>
-      <c r="D557" s="1"/>
-    </row>
-    <row r="558" spans="1:4">
-      <c r="A558" s="1"/>
-      <c r="D558" s="1"/>
-    </row>
-    <row r="559" spans="1:4">
-      <c r="A559" s="1"/>
-      <c r="D559" s="1"/>
-    </row>
-    <row r="560" spans="1:4">
-      <c r="A560" s="1"/>
-      <c r="D560" s="1"/>
-    </row>
-    <row r="561" spans="1:4">
-      <c r="A561" s="1"/>
-      <c r="D561" s="1"/>
-    </row>
-    <row r="562" spans="1:4">
-      <c r="A562" s="1"/>
-      <c r="D562" s="1"/>
-    </row>
-    <row r="563" spans="1:4">
-      <c r="A563" s="1"/>
-      <c r="D563" s="1"/>
-    </row>
-    <row r="564" spans="1:4">
-      <c r="A564" s="1"/>
-      <c r="D564" s="1"/>
+      <c r="A549" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="B549" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="D549" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" ht="58">
+      <c r="A550" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="B550" s="18" t="s">
+        <v>960</v>
+      </c>
+      <c r="C550" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D550" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" ht="58">
+      <c r="A551" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="B551" s="18" t="s">
+        <v>961</v>
+      </c>
+      <c r="C551" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D551" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" ht="58">
+      <c r="A552" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B552" s="18" t="s">
+        <v>963</v>
+      </c>
+      <c r="C552" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D552" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" ht="58">
+      <c r="A553" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="B553" s="18" t="s">
+        <v>963</v>
+      </c>
+      <c r="C553" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D553" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" ht="58">
+      <c r="A554" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="B554" s="18" t="s">
+        <v>965</v>
+      </c>
+      <c r="C554" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D554" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" ht="58">
+      <c r="A555" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="B555" s="18" t="s">
+        <v>965</v>
+      </c>
+      <c r="C555" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D555" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" ht="58">
+      <c r="A556" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="B556" s="18" t="s">
+        <v>965</v>
+      </c>
+      <c r="C556" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D556" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" ht="58">
+      <c r="A557" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B557" s="18" t="s">
+        <v>965</v>
+      </c>
+      <c r="C557" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D557" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" ht="58">
+      <c r="A558" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="B558" s="18" t="s">
+        <v>971</v>
+      </c>
+      <c r="C558" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D558" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" ht="58">
+      <c r="A559" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="B559" s="18" t="s">
+        <v>971</v>
+      </c>
+      <c r="C559" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D559" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" ht="58">
+      <c r="A560" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="B560" s="18" t="s">
+        <v>974</v>
+      </c>
+      <c r="C560" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D560" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" ht="58">
+      <c r="A561" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="B561" s="18" t="s">
+        <v>974</v>
+      </c>
+      <c r="C561" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D561" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" ht="58">
+      <c r="A562" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="B562" s="18" t="s">
+        <v>977</v>
+      </c>
+      <c r="C562" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D562" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" ht="58">
+      <c r="A563" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="B563" s="18" t="s">
+        <v>980</v>
+      </c>
+      <c r="C563" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D563" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" ht="58">
+      <c r="A564" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="B564" s="18" t="s">
+        <v>980</v>
+      </c>
+      <c r="C564" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D564" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="565" spans="1:4">
       <c r="A565" s="1"/>
@@ -49095,13 +49694,49 @@
       <c r="A9989" s="1"/>
       <c r="D9989" s="1"/>
     </row>
+    <row r="9990" spans="1:4">
+      <c r="A9990" s="1"/>
+      <c r="D9990" s="1"/>
+    </row>
+    <row r="9991" spans="1:4">
+      <c r="A9991" s="1"/>
+      <c r="D9991" s="1"/>
+    </row>
+    <row r="9992" spans="1:4">
+      <c r="A9992" s="1"/>
+      <c r="D9992" s="1"/>
+    </row>
+    <row r="9993" spans="1:4">
+      <c r="A9993" s="1"/>
+      <c r="D9993" s="1"/>
+    </row>
+    <row r="9994" spans="1:4">
+      <c r="A9994" s="1"/>
+      <c r="D9994" s="1"/>
+    </row>
+    <row r="9995" spans="1:4">
+      <c r="A9995" s="1"/>
+      <c r="D9995" s="1"/>
+    </row>
+    <row r="9996" spans="1:4">
+      <c r="A9996" s="1"/>
+      <c r="D9996" s="1"/>
+    </row>
+    <row r="9997" spans="1:4">
+      <c r="A9997" s="1"/>
+      <c r="D9997" s="1"/>
+    </row>
+    <row r="9998" spans="1:4">
+      <c r="A9998" s="1"/>
+      <c r="D9998" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D494" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D549"/>
   <mergeCells count="1">
-    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="H2:H10"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="G2:G8 G213:G239">
+  <conditionalFormatting sqref="G213:G239 G2:G10">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -49158,360 +49793,384 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$F$2:$F$9</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>$F$2:$F$10</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B24" display="https://alcon365.sharepoint.com/sites/alconfra/SitePages/MasterData.aspx?RootFolder=%2Fsites%2Falconfra%2FFinance%20Master%20Data%20Management%2FApproval%20Table%20Maintenance&amp;FolderCTID=0x012000F818F3CCE22AE94C86C3A970A6E10830&amp;View=%7B785A14CF-1D11-4535-" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B22" r:id="rId4" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B16" r:id="rId13" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FNew%20Global%20Travel%20%20Expense%20Policy%5FEffective%20August%201%202020%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B28" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B29" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B30" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B36" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B37" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B38" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B39" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B40" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B41" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B42" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B44" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B45" r:id="rId29" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B46" r:id="rId30" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B61" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B62" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B63" r:id="rId33" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2F%E7%B5%8C%E8%B2%BB%E7%B2%BE%E7%AE%97%E3%81%8A%E7%9F%A5%E3%82%89%E3%81%9B%E3%81%AE%E6%89%8B%E9%A0%86%E6%9B%B8%20V2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B65" r:id="rId34" display="https://alcon365.sharepoint.com/sites/InSight/096DocLib2/Forms/TheLensNameTitlePage.aspx?viewid=4a09b348%2D50df%2D46b7%2Da194%2D518047515835&amp;id=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations%2FTheLensPolicy%5Fen%2DEN%2Epdf&amp;parent=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B66" r:id="rId35" display="&quot;I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\02  T&amp;E\08  MAIL RELATED\FR0179446 - Flight ticket reimburse.msg&quot;" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B67" r:id="rId36" display="https://alcon365.sharepoint.com/sites/InSight/230DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG%2FHCP%E3%81%B8%E3%81%AE%E9%A3%B2%E9%A3%9F%E3%83%BB%E6%97%85%E8%B2%BB%E7%AD%89%E3%81%AE%E6%8F%90%E4%BE%9B%E4%B8%80%E8%A6%A7-%20%2020200801_final.pdf&amp;parent=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B68" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B69" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B70" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B71" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B72" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B73" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B99" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B100" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B101" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B102" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B103" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B104" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B105" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B106" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B107" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B108" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B109" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B111" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B112" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B114" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B115" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B116" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B117" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B118" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B119" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B120" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B121" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B122" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FAlcon%20Japan%20How%20to%20use%20expense%5F202101%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVI" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B113" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B123" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B124" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B125" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B126" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B127" r:id="rId69" display="https://alcon365.sharepoint.com/sites/InSight/SitePages/230/%E7%B2%BE%E7%AE%97%E3%81%A8%E9%80%8F%E6%98%8E%E6%80%A7%E3%82%AC%E3%82%A4%E3%83%89%E3%83%A9%E3%82%A4%E3%83%B3.aspx" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B128" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B110" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B129" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B130" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B131" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B132" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B133" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B134" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B135" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B136" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B137" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B138" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B139" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B140" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B141" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B142" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B143" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A146" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B147" r:id="rId88" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FVIM%2DVendor%20Invoice%20Management%20Upgrade%20May2021%5FRequester%20Approver%5FJapanese%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="B148" r:id="rId89" display="https://alcon365.sharepoint.com/:p:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B89D9BB48-49C8-4BC1-858C-0C99012AEC46%7D&amp;file=1-4-2.PO%E3%82%AD%E3%83%A3%E3%83%B3%E3%82%BB%E3%83%AB%E3%83%BB%E5%8F%96%E6%B6%88.pptx&amp;action=edit&amp;mobileredirect=true&amp;cid=93fd10e8-d2e3-48d6-8ad0-5cc94dc56304" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B149" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="B158" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B161" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="B162" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B168" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="B169" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B170" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="B171" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="B179" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="B181" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="B5" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="B6" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="B7" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="B23" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="B182" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="B183" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="B184" r:id="rId106" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B887C2330-A6E8-46B5-ACBA-F676866AD2D3%7D&amp;file=SRM%EF%BE%80%EF%BE%9E%EF%BD%B3%EF%BE%9D%EF%BE%8D%EF%BE%9F%EF%BD%B2%EF%BE%92%EF%BE%9D%EF%BE%84%EF%BE%98%EF%BD%B8%EF%BD%B4%EF%BD%BD%EF%BE%84_ver3.xlsx&amp;action=default&amp;mobileredirect=true" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="B185" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="B186" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="B187" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="B188" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="B189" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="B190" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="B191" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="B192" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="B193" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="B194" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="B197" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="B198" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="B199" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="B201" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="B202" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="B203" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="B204" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="B205" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="B206" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="B207" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="B208" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="B209" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="B210" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="B240" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="B241" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="B242" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="B243" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="B246" r:id="rId134" location="a-02" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="B247" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="B259" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="B264" r:id="rId137" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="B265" r:id="rId138" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="B266" r:id="rId139" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="B267" r:id="rId140" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="B274" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="B275" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="B276" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="B277" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="B278" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="B280" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="B281" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="B282" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="B283" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="B284" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="B285" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="B286" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="B287" r:id="rId153" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="B288" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="B289" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="B290" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="B291" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="B292" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="B293" r:id="rId159" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="B294" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="B295" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="B296" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="B297" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="B298" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="B299" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="B300" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="B301" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="B302" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="B303" r:id="rId169" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2F%E3%82%B0%E3%83%AD%E3%83%BC%E3%83%90%E3%83%AB%E7%89%88%E3%80%80%E3%82%A8%E3%83%B3%E3%83%89%E3%83%A6%E3%83%BC%E3%82%B6%E3%83%BCFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="B304" r:id="rId170" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%5FEnd%5FUser%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="B305" r:id="rId171" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FJA%5FGlobal%20TE%20policy%5FFAQ%2DR%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="B306" r:id="rId172" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FGlobal%20TE%20policy%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="B307" r:id="rId173" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%E3%83%A2%E3%83%90%E3%82%A4%E3%83%AB%E3%82%A2%E3%83%97%E3%83%AA%E3%83%87%E3%83%A2%2Ewebex&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides&amp;p=14" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="B308" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="B309" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="B310" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="B311" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="B312" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="B313" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="B314" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="B315" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="B316" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="B317" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="B318" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="B319" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="B320" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="B321" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="B322" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="B323" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="B324" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="B325" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="B326" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="B327" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="B328" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="B329" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="B330" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="B331" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="B332" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="B333" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="B334" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="B335" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="B336" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="B338" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="B339" r:id="rId204" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="B340" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="B343" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="B344" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="B345" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="B346" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="B347" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="B348" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="B349" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="B350" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="B351" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="B352" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="B353" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="B355" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="B356" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="B357" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="B358" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="B359" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="B360" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="B361" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="B362" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="B363" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="B364" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="B365" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="B366" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="B367" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="B368" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="B369" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="B370:B371" r:id="rId232" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\Withholding Tax\PSCへ提出_1110払源泉税.msg" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="B372" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="B373" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="B374" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="B375" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="B376" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="B377" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="B378" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="B379" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="B380" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="B381" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="B383" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="B384" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="B385" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="B386" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="B387" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="B388" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="B58" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="B57" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="B395" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="B396" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="B397" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="B398" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="B399" r:id="rId255" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="B400" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="B401" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="B402" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="B403" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="B405" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="B406" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="B407" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="B408" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="B409" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="B410" r:id="rId265" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="B411" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="B412" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="B413" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="B414" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="B415" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="B416" r:id="rId271" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="B417" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="B418" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="B419" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="B421" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="B429" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="B430" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="B431" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="B432" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="B433" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="B436" r:id="rId281" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="B437" r:id="rId282" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="B438" r:id="rId283" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="B439" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="B441" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="B442" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="B443" r:id="rId287" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="B444" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="B445" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="B446" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="B447" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="B448" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="B449" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="B450" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="B451" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="B452" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="B453" r:id="rId297" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="B454" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="B455" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="B456" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="B457" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="B458" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="B459" r:id="rId303" display="https://mdg.alcon.net/nwbc/?sap-client=010&amp;sap-language=EN&amp;sap-nwbc-context=03HM333035D633D53336000128D3C800C2350EF03304320D416C20C32DA3A4A4A0D84A5F3F37255D2F3127393F4F2F2FB5C4CAD2C0DC403FAF3C2959DFBE38B1403739273335AFC416A8410DC4CD49CC4B2F4D4C4FB575F50300&amp;sap-theme=sap_corbu&amp;sap-nwbc-node=0000000102" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="B460" r:id="rId304" display="https://grc.alcon.net/nwbc/?sap-nwbc-node=0000000005&amp;sap-nwbc-context=03HM333035D633D33336748AB232700E700F7274D675720C760D0D760D8A77F7718A3730307434303433802833303230360001E380101320D310C80400&amp;sap-client=010&amp;sap-language=JA&amp;sap-nwbc-history_item=&amp;sap-theme=sap_corbu" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="B461" r:id="rId305" location="ZMYBANK-display" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="B462" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="B463" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="B464" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="B465" r:id="rId309" display="maiko.okamoto@alcon.com" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="B467" r:id="rId310" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%20Table%20change%20request%20form%E8%A6%8B%E6%9C%AC%5F2021Nov%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="B468" r:id="rId311" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%5FTable%5FMaintence%5FRequest%5FForm%20%28002%29%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="B469" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="B471" r:id="rId313" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="B473" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="B474" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="B475" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="B476" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="B477" r:id="rId318" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="B478" r:id="rId319" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="B479" r:id="rId320" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="B480" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="B484" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="B485" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="B486" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="B487" r:id="rId325" location="/site/FRAGlobal/workbooks/8033/views" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="B488" r:id="rId326" location="/site/FRAGlobal/workbooks/8033/views" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="B489" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="B490" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="B491" r:id="rId329" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="B492" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="B493" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="B494" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="B498" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="B500" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="B501" r:id="rId335" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="B506" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="B519" r:id="rId337" xr:uid="{F720CA53-E902-4015-99E7-CF7ED36AC79D}"/>
-    <hyperlink ref="B521" r:id="rId338" xr:uid="{3CCDE37B-D158-43AD-A978-3B78F9D9BA39}"/>
-    <hyperlink ref="B522" r:id="rId339" xr:uid="{ADF26670-EF5D-48BD-A644-A0CF8811E942}"/>
-    <hyperlink ref="B523" r:id="rId340" xr:uid="{7555B120-F5B3-469E-A7E2-CA5642A357B9}"/>
-    <hyperlink ref="B525" r:id="rId341" display="http://alusfw-sp353107.alcon.net/NimbusFinance/CtrlWebISAPI.dll/app/diagram/0:9B906E1EB57A44FB8CF3F2821EA071DE" xr:uid="{CAEC30DB-069F-48E1-9F54-0FE5126ED1C6}"/>
+    <hyperlink ref="B18" r:id="rId1"/>
+    <hyperlink ref="B24" display="https://alcon365.sharepoint.com/sites/alconfra/SitePages/MasterData.aspx?RootFolder=%2Fsites%2Falconfra%2FFinance%20Master%20Data%20Management%2FApproval%20Table%20Maintenance&amp;FolderCTID=0x012000F818F3CCE22AE94C86C3A970A6E10830&amp;View=%7B785A14CF-1D11-4535-"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId3"/>
+    <hyperlink ref="B22" r:id="rId4" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1"/>
+    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B13" r:id="rId10"/>
+    <hyperlink ref="B14" r:id="rId11"/>
+    <hyperlink ref="B15" r:id="rId12"/>
+    <hyperlink ref="B16" r:id="rId13" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FNew%20Global%20Travel%20%20Expense%20Policy%5FEffective%20August%201%202020%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents"/>
+    <hyperlink ref="B17" r:id="rId14"/>
+    <hyperlink ref="B28" r:id="rId15"/>
+    <hyperlink ref="B29" r:id="rId16"/>
+    <hyperlink ref="B30" r:id="rId17"/>
+    <hyperlink ref="B31" r:id="rId18"/>
+    <hyperlink ref="B33" r:id="rId19"/>
+    <hyperlink ref="B34" r:id="rId20"/>
+    <hyperlink ref="B36" r:id="rId21"/>
+    <hyperlink ref="B37" r:id="rId22"/>
+    <hyperlink ref="B38" r:id="rId23"/>
+    <hyperlink ref="B39" r:id="rId24"/>
+    <hyperlink ref="B40" r:id="rId25"/>
+    <hyperlink ref="B41" r:id="rId26"/>
+    <hyperlink ref="B42" r:id="rId27"/>
+    <hyperlink ref="B44" r:id="rId28"/>
+    <hyperlink ref="B45" r:id="rId29" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021"/>
+    <hyperlink ref="B46" r:id="rId30" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021"/>
+    <hyperlink ref="B61" r:id="rId31"/>
+    <hyperlink ref="B62" r:id="rId32"/>
+    <hyperlink ref="B63" r:id="rId33" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2F%E7%B5%8C%E8%B2%BB%E7%B2%BE%E7%AE%97%E3%81%8A%E7%9F%A5%E3%82%89%E3%81%9B%E3%81%AE%E6%89%8B%E9%A0%86%E6%9B%B8%20V2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs"/>
+    <hyperlink ref="B65" r:id="rId34" display="https://alcon365.sharepoint.com/sites/InSight/096DocLib2/Forms/TheLensNameTitlePage.aspx?viewid=4a09b348%2D50df%2D46b7%2Da194%2D518047515835&amp;id=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations%2FTheLensPolicy%5Fen%2DEN%2Epdf&amp;parent=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations"/>
+    <hyperlink ref="B66" r:id="rId35" display="&quot;I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\02  T&amp;E\08  MAIL RELATED\FR0179446 - Flight ticket reimburse.msg&quot;"/>
+    <hyperlink ref="B67" r:id="rId36" display="https://alcon365.sharepoint.com/sites/InSight/230DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG%2FHCP%E3%81%B8%E3%81%AE%E9%A3%B2%E9%A3%9F%E3%83%BB%E6%97%85%E8%B2%BB%E7%AD%89%E3%81%AE%E6%8F%90%E4%BE%9B%E4%B8%80%E8%A6%A7-%20%2020200801_final.pdf&amp;parent=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG"/>
+    <hyperlink ref="B68" r:id="rId37"/>
+    <hyperlink ref="B69" r:id="rId38"/>
+    <hyperlink ref="B70" r:id="rId39"/>
+    <hyperlink ref="B71" r:id="rId40"/>
+    <hyperlink ref="B72" r:id="rId41"/>
+    <hyperlink ref="B73" r:id="rId42"/>
+    <hyperlink ref="B99" r:id="rId43"/>
+    <hyperlink ref="B100" r:id="rId44"/>
+    <hyperlink ref="B101" r:id="rId45"/>
+    <hyperlink ref="B102" r:id="rId46"/>
+    <hyperlink ref="B103" r:id="rId47"/>
+    <hyperlink ref="B104" r:id="rId48"/>
+    <hyperlink ref="B105" r:id="rId49"/>
+    <hyperlink ref="B106" r:id="rId50"/>
+    <hyperlink ref="B107" r:id="rId51"/>
+    <hyperlink ref="B108" r:id="rId52"/>
+    <hyperlink ref="B109" r:id="rId53"/>
+    <hyperlink ref="B111" r:id="rId54"/>
+    <hyperlink ref="B112" r:id="rId55"/>
+    <hyperlink ref="B114" r:id="rId56"/>
+    <hyperlink ref="B115" r:id="rId57"/>
+    <hyperlink ref="B116" r:id="rId58"/>
+    <hyperlink ref="B117" r:id="rId59"/>
+    <hyperlink ref="B118" r:id="rId60"/>
+    <hyperlink ref="B119" r:id="rId61"/>
+    <hyperlink ref="B120" r:id="rId62"/>
+    <hyperlink ref="B121" r:id="rId63"/>
+    <hyperlink ref="B122" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FAlcon%20Japan%20How%20to%20use%20expense%5F202101%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVI"/>
+    <hyperlink ref="B113" r:id="rId64"/>
+    <hyperlink ref="B123" r:id="rId65"/>
+    <hyperlink ref="B124" r:id="rId66"/>
+    <hyperlink ref="B125" r:id="rId67"/>
+    <hyperlink ref="B126" r:id="rId68"/>
+    <hyperlink ref="B127" r:id="rId69" display="https://alcon365.sharepoint.com/sites/InSight/SitePages/230/%E7%B2%BE%E7%AE%97%E3%81%A8%E9%80%8F%E6%98%8E%E6%80%A7%E3%82%AC%E3%82%A4%E3%83%89%E3%83%A9%E3%82%A4%E3%83%B3.aspx"/>
+    <hyperlink ref="B128" r:id="rId70"/>
+    <hyperlink ref="B110" r:id="rId71"/>
+    <hyperlink ref="B129" r:id="rId72"/>
+    <hyperlink ref="B130" r:id="rId73"/>
+    <hyperlink ref="B131" r:id="rId74"/>
+    <hyperlink ref="B132" r:id="rId75"/>
+    <hyperlink ref="B133" r:id="rId76"/>
+    <hyperlink ref="B134" r:id="rId77"/>
+    <hyperlink ref="B135" r:id="rId78"/>
+    <hyperlink ref="B136" r:id="rId79"/>
+    <hyperlink ref="B137" r:id="rId80"/>
+    <hyperlink ref="B138" r:id="rId81"/>
+    <hyperlink ref="B139" r:id="rId82"/>
+    <hyperlink ref="B140" r:id="rId83"/>
+    <hyperlink ref="B141" r:id="rId84"/>
+    <hyperlink ref="B142" r:id="rId85"/>
+    <hyperlink ref="B143" r:id="rId86"/>
+    <hyperlink ref="A146" r:id="rId87"/>
+    <hyperlink ref="B147" r:id="rId88" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FVIM%2DVendor%20Invoice%20Management%20Upgrade%20May2021%5FRequester%20Approver%5FJapanese%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM"/>
+    <hyperlink ref="B148" r:id="rId89" display="https://alcon365.sharepoint.com/:p:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B89D9BB48-49C8-4BC1-858C-0C99012AEC46%7D&amp;file=1-4-2.PO%E3%82%AD%E3%83%A3%E3%83%B3%E3%82%BB%E3%83%AB%E3%83%BB%E5%8F%96%E6%B6%88.pptx&amp;action=edit&amp;mobileredirect=true&amp;cid=93fd10e8-d2e3-48d6-8ad0-5cc94dc56304"/>
+    <hyperlink ref="B149" r:id="rId90"/>
+    <hyperlink ref="B158" r:id="rId91"/>
+    <hyperlink ref="B161" r:id="rId92"/>
+    <hyperlink ref="B162" r:id="rId93"/>
+    <hyperlink ref="B168" r:id="rId94"/>
+    <hyperlink ref="B169" r:id="rId95"/>
+    <hyperlink ref="B170" r:id="rId96"/>
+    <hyperlink ref="B171" r:id="rId97"/>
+    <hyperlink ref="B179" r:id="rId98"/>
+    <hyperlink ref="B181" r:id="rId99"/>
+    <hyperlink ref="B5" r:id="rId100"/>
+    <hyperlink ref="B6" r:id="rId101"/>
+    <hyperlink ref="B7" r:id="rId102"/>
+    <hyperlink ref="B23" r:id="rId103"/>
+    <hyperlink ref="B182" r:id="rId104"/>
+    <hyperlink ref="B183" r:id="rId105"/>
+    <hyperlink ref="B184" r:id="rId106" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B887C2330-A6E8-46B5-ACBA-F676866AD2D3%7D&amp;file=SRM%EF%BE%80%EF%BE%9E%EF%BD%B3%EF%BE%9D%EF%BE%8D%EF%BE%9F%EF%BD%B2%EF%BE%92%EF%BE%9D%EF%BE%84%EF%BE%98%EF%BD%B8%EF%BD%B4%EF%BD%BD%EF%BE%84_ver3.xlsx&amp;action=default&amp;mobileredirect=true"/>
+    <hyperlink ref="B185" r:id="rId107"/>
+    <hyperlink ref="B186" r:id="rId108"/>
+    <hyperlink ref="B187" r:id="rId109"/>
+    <hyperlink ref="B188" r:id="rId110"/>
+    <hyperlink ref="B189" r:id="rId111"/>
+    <hyperlink ref="B190" r:id="rId112"/>
+    <hyperlink ref="B191" r:id="rId113"/>
+    <hyperlink ref="B192" r:id="rId114"/>
+    <hyperlink ref="B193" r:id="rId115"/>
+    <hyperlink ref="B194" r:id="rId116"/>
+    <hyperlink ref="B197" r:id="rId117"/>
+    <hyperlink ref="B198" r:id="rId118"/>
+    <hyperlink ref="B199" r:id="rId119"/>
+    <hyperlink ref="B201" r:id="rId120"/>
+    <hyperlink ref="B202" r:id="rId121"/>
+    <hyperlink ref="B203" r:id="rId122"/>
+    <hyperlink ref="B204" r:id="rId123"/>
+    <hyperlink ref="B205" r:id="rId124"/>
+    <hyperlink ref="B206" r:id="rId125"/>
+    <hyperlink ref="B207" r:id="rId126"/>
+    <hyperlink ref="B208" r:id="rId127"/>
+    <hyperlink ref="B209" r:id="rId128"/>
+    <hyperlink ref="B210" r:id="rId129"/>
+    <hyperlink ref="B240" r:id="rId130"/>
+    <hyperlink ref="B241" r:id="rId131"/>
+    <hyperlink ref="B242" r:id="rId132"/>
+    <hyperlink ref="B243" r:id="rId133"/>
+    <hyperlink ref="B246" r:id="rId134" location="a-02"/>
+    <hyperlink ref="B247" r:id="rId135"/>
+    <hyperlink ref="B259" r:id="rId136"/>
+    <hyperlink ref="B264" r:id="rId137" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
+    <hyperlink ref="B265" r:id="rId138" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
+    <hyperlink ref="B266" r:id="rId139" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
+    <hyperlink ref="B267" r:id="rId140" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
+    <hyperlink ref="B274" r:id="rId141"/>
+    <hyperlink ref="B275" r:id="rId142"/>
+    <hyperlink ref="B276" r:id="rId143"/>
+    <hyperlink ref="B277" r:id="rId144"/>
+    <hyperlink ref="B278" r:id="rId145"/>
+    <hyperlink ref="B280" r:id="rId146"/>
+    <hyperlink ref="B281" r:id="rId147"/>
+    <hyperlink ref="B282" r:id="rId148"/>
+    <hyperlink ref="B283" r:id="rId149"/>
+    <hyperlink ref="B284" r:id="rId150"/>
+    <hyperlink ref="B285" r:id="rId151"/>
+    <hyperlink ref="B286" r:id="rId152"/>
+    <hyperlink ref="B287" r:id="rId153"/>
+    <hyperlink ref="B288" r:id="rId154"/>
+    <hyperlink ref="B289" r:id="rId155"/>
+    <hyperlink ref="B290" r:id="rId156"/>
+    <hyperlink ref="B291" r:id="rId157"/>
+    <hyperlink ref="B292" r:id="rId158"/>
+    <hyperlink ref="B293" r:id="rId159"/>
+    <hyperlink ref="B294" r:id="rId160"/>
+    <hyperlink ref="B295" r:id="rId161"/>
+    <hyperlink ref="B296" r:id="rId162"/>
+    <hyperlink ref="B297" r:id="rId163"/>
+    <hyperlink ref="B298" r:id="rId164"/>
+    <hyperlink ref="B299" r:id="rId165"/>
+    <hyperlink ref="B300" r:id="rId166"/>
+    <hyperlink ref="B301" r:id="rId167"/>
+    <hyperlink ref="B302" r:id="rId168"/>
+    <hyperlink ref="B303" r:id="rId169" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2F%E3%82%B0%E3%83%AD%E3%83%BC%E3%83%90%E3%83%AB%E7%89%88%E3%80%80%E3%82%A8%E3%83%B3%E3%83%89%E3%83%A6%E3%83%BC%E3%82%B6%E3%83%BCFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
+    <hyperlink ref="B304" r:id="rId170" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%5FEnd%5FUser%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
+    <hyperlink ref="B305" r:id="rId171" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FJA%5FGlobal%20TE%20policy%5FFAQ%2DR%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs"/>
+    <hyperlink ref="B306" r:id="rId172" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FGlobal%20TE%20policy%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs"/>
+    <hyperlink ref="B307" r:id="rId173" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%E3%83%A2%E3%83%90%E3%82%A4%E3%83%AB%E3%82%A2%E3%83%97%E3%83%AA%E3%83%87%E3%83%A2%2Ewebex&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides&amp;p=14"/>
+    <hyperlink ref="B308" r:id="rId174"/>
+    <hyperlink ref="B309" r:id="rId175"/>
+    <hyperlink ref="B310" r:id="rId176"/>
+    <hyperlink ref="B311" r:id="rId177"/>
+    <hyperlink ref="B312" r:id="rId178"/>
+    <hyperlink ref="B313" r:id="rId179"/>
+    <hyperlink ref="B314" r:id="rId180"/>
+    <hyperlink ref="B315" r:id="rId181"/>
+    <hyperlink ref="B316" r:id="rId182"/>
+    <hyperlink ref="B317" r:id="rId183"/>
+    <hyperlink ref="B318" r:id="rId184"/>
+    <hyperlink ref="B319" r:id="rId185"/>
+    <hyperlink ref="B320" r:id="rId186"/>
+    <hyperlink ref="B321" r:id="rId187"/>
+    <hyperlink ref="B322" r:id="rId188"/>
+    <hyperlink ref="B323" r:id="rId189"/>
+    <hyperlink ref="B324" r:id="rId190"/>
+    <hyperlink ref="B325" r:id="rId191"/>
+    <hyperlink ref="B326" r:id="rId192"/>
+    <hyperlink ref="B327" r:id="rId193"/>
+    <hyperlink ref="B328" r:id="rId194"/>
+    <hyperlink ref="B329" r:id="rId195"/>
+    <hyperlink ref="B330" r:id="rId196"/>
+    <hyperlink ref="B331" r:id="rId197"/>
+    <hyperlink ref="B332" r:id="rId198"/>
+    <hyperlink ref="B333" r:id="rId199"/>
+    <hyperlink ref="B334" r:id="rId200"/>
+    <hyperlink ref="B335" r:id="rId201"/>
+    <hyperlink ref="B336" r:id="rId202"/>
+    <hyperlink ref="B338" r:id="rId203"/>
+    <hyperlink ref="B339" r:id="rId204" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1"/>
+    <hyperlink ref="B340" r:id="rId205"/>
+    <hyperlink ref="B343" r:id="rId206"/>
+    <hyperlink ref="B344" r:id="rId207"/>
+    <hyperlink ref="B345" r:id="rId208"/>
+    <hyperlink ref="B346" r:id="rId209"/>
+    <hyperlink ref="B347" r:id="rId210"/>
+    <hyperlink ref="B348" r:id="rId211"/>
+    <hyperlink ref="B349" r:id="rId212"/>
+    <hyperlink ref="B350" r:id="rId213"/>
+    <hyperlink ref="B351" r:id="rId214"/>
+    <hyperlink ref="B352" r:id="rId215"/>
+    <hyperlink ref="B353" r:id="rId216"/>
+    <hyperlink ref="B355" r:id="rId217"/>
+    <hyperlink ref="B356" r:id="rId218"/>
+    <hyperlink ref="B357" r:id="rId219"/>
+    <hyperlink ref="B358" r:id="rId220"/>
+    <hyperlink ref="B359" r:id="rId221"/>
+    <hyperlink ref="B360" r:id="rId222"/>
+    <hyperlink ref="B361" r:id="rId223"/>
+    <hyperlink ref="B362" r:id="rId224"/>
+    <hyperlink ref="B363" r:id="rId225"/>
+    <hyperlink ref="B364" r:id="rId226"/>
+    <hyperlink ref="B365" r:id="rId227"/>
+    <hyperlink ref="B366" r:id="rId228"/>
+    <hyperlink ref="B367" r:id="rId229"/>
+    <hyperlink ref="B368" r:id="rId230"/>
+    <hyperlink ref="B369" r:id="rId231"/>
+    <hyperlink ref="B370:B371" r:id="rId232" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\Withholding Tax\PSCへ提出_1110払源泉税.msg"/>
+    <hyperlink ref="B372" r:id="rId233"/>
+    <hyperlink ref="B373" r:id="rId234"/>
+    <hyperlink ref="B374" r:id="rId235"/>
+    <hyperlink ref="B375" r:id="rId236"/>
+    <hyperlink ref="B376" r:id="rId237"/>
+    <hyperlink ref="B377" r:id="rId238"/>
+    <hyperlink ref="B378" r:id="rId239"/>
+    <hyperlink ref="B379" r:id="rId240"/>
+    <hyperlink ref="B380" r:id="rId241"/>
+    <hyperlink ref="B381" r:id="rId242"/>
+    <hyperlink ref="B383" r:id="rId243"/>
+    <hyperlink ref="B384" r:id="rId244"/>
+    <hyperlink ref="B385" r:id="rId245"/>
+    <hyperlink ref="B386" r:id="rId246"/>
+    <hyperlink ref="B387" r:id="rId247"/>
+    <hyperlink ref="B388" r:id="rId248"/>
+    <hyperlink ref="B58" r:id="rId249"/>
+    <hyperlink ref="B57" r:id="rId250"/>
+    <hyperlink ref="B395" r:id="rId251"/>
+    <hyperlink ref="B396" r:id="rId252"/>
+    <hyperlink ref="B397" r:id="rId253"/>
+    <hyperlink ref="B398" r:id="rId254"/>
+    <hyperlink ref="B399" r:id="rId255"/>
+    <hyperlink ref="B400" r:id="rId256"/>
+    <hyperlink ref="B401" r:id="rId257"/>
+    <hyperlink ref="B402" r:id="rId258"/>
+    <hyperlink ref="B403" r:id="rId259"/>
+    <hyperlink ref="B405" r:id="rId260"/>
+    <hyperlink ref="B406" r:id="rId261"/>
+    <hyperlink ref="B407" r:id="rId262"/>
+    <hyperlink ref="B408" r:id="rId263"/>
+    <hyperlink ref="B409" r:id="rId264"/>
+    <hyperlink ref="B410" r:id="rId265"/>
+    <hyperlink ref="B411" r:id="rId266"/>
+    <hyperlink ref="B412" r:id="rId267"/>
+    <hyperlink ref="B413" r:id="rId268"/>
+    <hyperlink ref="B414" r:id="rId269"/>
+    <hyperlink ref="B415" r:id="rId270"/>
+    <hyperlink ref="B416" r:id="rId271"/>
+    <hyperlink ref="B417" r:id="rId272"/>
+    <hyperlink ref="B418" r:id="rId273"/>
+    <hyperlink ref="B419" r:id="rId274"/>
+    <hyperlink ref="B421" r:id="rId275"/>
+    <hyperlink ref="B429" r:id="rId276"/>
+    <hyperlink ref="B430" r:id="rId277"/>
+    <hyperlink ref="B431" r:id="rId278"/>
+    <hyperlink ref="B432" r:id="rId279"/>
+    <hyperlink ref="B433" r:id="rId280"/>
+    <hyperlink ref="B436" r:id="rId281" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday"/>
+    <hyperlink ref="B437" r:id="rId282" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday"/>
+    <hyperlink ref="B438" r:id="rId283" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday"/>
+    <hyperlink ref="B439" r:id="rId284"/>
+    <hyperlink ref="B441" r:id="rId285"/>
+    <hyperlink ref="B442" r:id="rId286"/>
+    <hyperlink ref="B443" r:id="rId287"/>
+    <hyperlink ref="B444" r:id="rId288"/>
+    <hyperlink ref="B445" r:id="rId289"/>
+    <hyperlink ref="B446" r:id="rId290"/>
+    <hyperlink ref="B447" r:id="rId291"/>
+    <hyperlink ref="B448" r:id="rId292"/>
+    <hyperlink ref="B449" r:id="rId293"/>
+    <hyperlink ref="B450" r:id="rId294"/>
+    <hyperlink ref="B451" r:id="rId295"/>
+    <hyperlink ref="B452" r:id="rId296"/>
+    <hyperlink ref="B453" r:id="rId297"/>
+    <hyperlink ref="B454" r:id="rId298"/>
+    <hyperlink ref="B455" r:id="rId299"/>
+    <hyperlink ref="B456" r:id="rId300"/>
+    <hyperlink ref="B457" r:id="rId301"/>
+    <hyperlink ref="B458" r:id="rId302"/>
+    <hyperlink ref="B459" r:id="rId303" display="https://mdg.alcon.net/nwbc/?sap-client=010&amp;sap-language=EN&amp;sap-nwbc-context=03HM333035D633D53336000128D3C800C2350EF03304320D416C20C32DA3A4A4A0D84A5F3F37255D2F3127393F4F2F2FB5C4CAD2C0DC403FAF3C2959DFBE38B1403739273335AFC416A8410DC4CD49CC4B2F4D4C4FB575F50300&amp;sap-theme=sap_corbu&amp;sap-nwbc-node=0000000102"/>
+    <hyperlink ref="B460" r:id="rId304" display="https://grc.alcon.net/nwbc/?sap-nwbc-node=0000000005&amp;sap-nwbc-context=03HM333035D633D33336748AB232700E700F7274D675720C760D0D760D8A77F7718A3730307434303433802833303230360001E380101320D310C80400&amp;sap-client=010&amp;sap-language=JA&amp;sap-nwbc-history_item=&amp;sap-theme=sap_corbu"/>
+    <hyperlink ref="B461" r:id="rId305" location="ZMYBANK-display"/>
+    <hyperlink ref="B462" r:id="rId306"/>
+    <hyperlink ref="B463" r:id="rId307"/>
+    <hyperlink ref="B464" r:id="rId308"/>
+    <hyperlink ref="B465" r:id="rId309" display="maiko.okamoto@alcon.com"/>
+    <hyperlink ref="B467" r:id="rId310" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%20Table%20change%20request%20form%E8%A6%8B%E6%9C%AC%5F2021Nov%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM"/>
+    <hyperlink ref="B468" r:id="rId311" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%5FTable%5FMaintence%5FRequest%5FForm%20%28002%29%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM"/>
+    <hyperlink ref="B469" r:id="rId312"/>
+    <hyperlink ref="B471" r:id="rId313"/>
+    <hyperlink ref="B473" r:id="rId314"/>
+    <hyperlink ref="B474" r:id="rId315"/>
+    <hyperlink ref="B475" r:id="rId316"/>
+    <hyperlink ref="B476" r:id="rId317"/>
+    <hyperlink ref="B477" r:id="rId318" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
+    <hyperlink ref="B478" r:id="rId319" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents"/>
+    <hyperlink ref="B479" r:id="rId320" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents"/>
+    <hyperlink ref="B480" r:id="rId321"/>
+    <hyperlink ref="B484" r:id="rId322"/>
+    <hyperlink ref="B485" r:id="rId323"/>
+    <hyperlink ref="B486" r:id="rId324"/>
+    <hyperlink ref="B487" r:id="rId325" location="/site/FRAGlobal/workbooks/8033/views"/>
+    <hyperlink ref="B488" r:id="rId326" location="/site/FRAGlobal/workbooks/8033/views"/>
+    <hyperlink ref="B489" r:id="rId327"/>
+    <hyperlink ref="B490" r:id="rId328"/>
+    <hyperlink ref="B491" r:id="rId329"/>
+    <hyperlink ref="B492" r:id="rId330"/>
+    <hyperlink ref="B493" r:id="rId331"/>
+    <hyperlink ref="B494" r:id="rId332"/>
+    <hyperlink ref="B498" r:id="rId333"/>
+    <hyperlink ref="B500" r:id="rId334"/>
+    <hyperlink ref="B501" r:id="rId335"/>
+    <hyperlink ref="B506" r:id="rId336"/>
+    <hyperlink ref="B519" r:id="rId337"/>
+    <hyperlink ref="B521" r:id="rId338"/>
+    <hyperlink ref="B522" r:id="rId339"/>
+    <hyperlink ref="B523" r:id="rId340"/>
+    <hyperlink ref="B525" r:id="rId341" display="http://alusfw-sp353107.alcon.net/NimbusFinance/CtrlWebISAPI.dll/app/diagram/0:9B906E1EB57A44FB8CF3F2821EA071DE"/>
+    <hyperlink ref="B526" r:id="rId342"/>
+    <hyperlink ref="B539" r:id="rId343"/>
+    <hyperlink ref="B540" r:id="rId344"/>
+    <hyperlink ref="B541" r:id="rId345"/>
+    <hyperlink ref="B543" r:id="rId346"/>
+    <hyperlink ref="B542" r:id="rId347"/>
+    <hyperlink ref="B544" r:id="rId348"/>
+    <hyperlink ref="B546" r:id="rId349"/>
+    <hyperlink ref="B547" r:id="rId350"/>
+    <hyperlink ref="B550" r:id="rId351"/>
+    <hyperlink ref="B551" r:id="rId352"/>
+    <hyperlink ref="B552" r:id="rId353"/>
+    <hyperlink ref="B553" r:id="rId354"/>
+    <hyperlink ref="B554" r:id="rId355"/>
+    <hyperlink ref="B555" r:id="rId356"/>
+    <hyperlink ref="B556" r:id="rId357"/>
+    <hyperlink ref="B557" r:id="rId358"/>
+    <hyperlink ref="B558" r:id="rId359"/>
+    <hyperlink ref="B559" r:id="rId360"/>
+    <hyperlink ref="B560" r:id="rId361"/>
+    <hyperlink ref="B561" r:id="rId362"/>
+    <hyperlink ref="B562" r:id="rId363"/>
+    <hyperlink ref="B563" r:id="rId364"/>
+    <hyperlink ref="B564" r:id="rId365"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId342"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId366"/>
   <customProperties>
-    <customPr name="_pios_id" r:id="rId343"/>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId344"/>
+    <customPr name="_pios_id" r:id="rId367"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId368"/>
   </customProperties>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -49531,7 +50190,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G2:G8 G213:G239</xm:sqref>
+          <xm:sqref>G213:G239 G2:G10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3FB01497-E984-4BAD-A8F7-39415467035E}">
@@ -49588,7 +50247,7 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Category!$A$2:$A$25</xm:f>
           </x14:formula1>
@@ -49601,10 +50260,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -49738,13 +50399,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <customProperties>
     <customPr name="_pios_id" r:id="rId2"/>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -49830,14 +50490,13 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <customProperties>
     <customPr name="_pios_id" r:id="rId3"/>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId4"/>
   </customProperties>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit v2 Feb 23rd
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656C683E-F658-45EE-AB46-55DE51431C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$H$657</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="1182">
   <si>
     <t>Kota</t>
     <phoneticPr fontId="2"/>
@@ -3946,7 +3947,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16">
     <font>
       <sz val="11"/>
@@ -4612,14 +4613,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="C662" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="11" topLeftCell="C660" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="G670" sqref="G670"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -12743,7 +12744,9 @@
       <c r="A570" s="1" t="s">
         <v>987</v>
       </c>
-      <c r="B570" s="3"/>
+      <c r="B570" s="3" t="s">
+        <v>852</v>
+      </c>
       <c r="C570" s="2" t="s">
         <v>199</v>
       </c>
@@ -51504,7 +51507,7 @@
       <c r="D9998" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H657"/>
+  <autoFilter ref="A1:H657" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="H2:H11"/>
   </mergeCells>
@@ -51566,432 +51569,432 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D613 D617:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D613 D617:D1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$F$2:$F$11</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1"/>
-    <hyperlink ref="B24" display="https://alcon365.sharepoint.com/sites/alconfra/SitePages/MasterData.aspx?RootFolder=%2Fsites%2Falconfra%2FFinance%20Master%20Data%20Management%2FApproval%20Table%20Maintenance&amp;FolderCTID=0x012000F818F3CCE22AE94C86C3A970A6E10830&amp;View=%7B785A14CF-1D11-4535-"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B19" r:id="rId3"/>
-    <hyperlink ref="B22" r:id="rId4" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B13" r:id="rId10"/>
-    <hyperlink ref="B14" r:id="rId11"/>
-    <hyperlink ref="B15" r:id="rId12"/>
-    <hyperlink ref="B16" r:id="rId13" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FNew%20Global%20Travel%20%20Expense%20Policy%5FEffective%20August%201%202020%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents"/>
-    <hyperlink ref="B17" r:id="rId14"/>
-    <hyperlink ref="B28" r:id="rId15"/>
-    <hyperlink ref="B29" r:id="rId16"/>
-    <hyperlink ref="B30" r:id="rId17"/>
-    <hyperlink ref="B31" r:id="rId18"/>
-    <hyperlink ref="B33" r:id="rId19"/>
-    <hyperlink ref="B34" r:id="rId20"/>
-    <hyperlink ref="B36" r:id="rId21"/>
-    <hyperlink ref="B37" r:id="rId22"/>
-    <hyperlink ref="B38" r:id="rId23"/>
-    <hyperlink ref="B39" r:id="rId24"/>
-    <hyperlink ref="B40" r:id="rId25"/>
-    <hyperlink ref="B41" r:id="rId26"/>
-    <hyperlink ref="B42" r:id="rId27"/>
-    <hyperlink ref="B44" r:id="rId28"/>
-    <hyperlink ref="B45" r:id="rId29" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021"/>
-    <hyperlink ref="B46" r:id="rId30" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021"/>
-    <hyperlink ref="B61" r:id="rId31"/>
-    <hyperlink ref="B62" r:id="rId32"/>
-    <hyperlink ref="B63" r:id="rId33" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2F%E7%B5%8C%E8%B2%BB%E7%B2%BE%E7%AE%97%E3%81%8A%E7%9F%A5%E3%82%89%E3%81%9B%E3%81%AE%E6%89%8B%E9%A0%86%E6%9B%B8%20V2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs"/>
-    <hyperlink ref="B65" r:id="rId34" display="https://alcon365.sharepoint.com/sites/InSight/096DocLib2/Forms/TheLensNameTitlePage.aspx?viewid=4a09b348%2D50df%2D46b7%2Da194%2D518047515835&amp;id=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations%2FTheLensPolicy%5Fen%2DEN%2Epdf&amp;parent=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations"/>
-    <hyperlink ref="B67" r:id="rId35" display="https://alcon365.sharepoint.com/sites/InSight/230DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG%2FHCP%E3%81%B8%E3%81%AE%E9%A3%B2%E9%A3%9F%E3%83%BB%E6%97%85%E8%B2%BB%E7%AD%89%E3%81%AE%E6%8F%90%E4%BE%9B%E4%B8%80%E8%A6%A7-%20%2020200801_final.pdf&amp;parent=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG"/>
-    <hyperlink ref="B68" r:id="rId36"/>
-    <hyperlink ref="B69" r:id="rId37"/>
-    <hyperlink ref="B70" r:id="rId38"/>
-    <hyperlink ref="B71" r:id="rId39"/>
-    <hyperlink ref="B72" r:id="rId40"/>
-    <hyperlink ref="B73" r:id="rId41"/>
-    <hyperlink ref="B99" r:id="rId42"/>
-    <hyperlink ref="B100" r:id="rId43"/>
-    <hyperlink ref="B101" r:id="rId44"/>
-    <hyperlink ref="B102" r:id="rId45"/>
-    <hyperlink ref="B103" r:id="rId46"/>
-    <hyperlink ref="B104" r:id="rId47"/>
-    <hyperlink ref="B105" r:id="rId48"/>
-    <hyperlink ref="B106" r:id="rId49"/>
-    <hyperlink ref="B107" r:id="rId50"/>
-    <hyperlink ref="B108" r:id="rId51"/>
-    <hyperlink ref="B109" r:id="rId52"/>
-    <hyperlink ref="B111" r:id="rId53"/>
-    <hyperlink ref="B112" r:id="rId54"/>
-    <hyperlink ref="B114" r:id="rId55"/>
-    <hyperlink ref="B115" r:id="rId56"/>
-    <hyperlink ref="B116" r:id="rId57"/>
-    <hyperlink ref="B117" r:id="rId58"/>
-    <hyperlink ref="B118" r:id="rId59"/>
-    <hyperlink ref="B119" r:id="rId60"/>
-    <hyperlink ref="B120" r:id="rId61"/>
-    <hyperlink ref="B121" r:id="rId62"/>
-    <hyperlink ref="B122" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FAlcon%20Japan%20How%20to%20use%20expense%5F202101%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVI"/>
-    <hyperlink ref="B113" r:id="rId63"/>
-    <hyperlink ref="B123" r:id="rId64"/>
-    <hyperlink ref="B124" r:id="rId65"/>
-    <hyperlink ref="B125" r:id="rId66"/>
-    <hyperlink ref="B126" r:id="rId67"/>
-    <hyperlink ref="B127" r:id="rId68" display="https://alcon365.sharepoint.com/sites/InSight/SitePages/230/%E7%B2%BE%E7%AE%97%E3%81%A8%E9%80%8F%E6%98%8E%E6%80%A7%E3%82%AC%E3%82%A4%E3%83%89%E3%83%A9%E3%82%A4%E3%83%B3.aspx"/>
-    <hyperlink ref="B128" r:id="rId69"/>
-    <hyperlink ref="B110" r:id="rId70"/>
-    <hyperlink ref="B129" r:id="rId71"/>
-    <hyperlink ref="B130" r:id="rId72"/>
-    <hyperlink ref="B131" r:id="rId73"/>
-    <hyperlink ref="B132" r:id="rId74"/>
-    <hyperlink ref="B133" r:id="rId75"/>
-    <hyperlink ref="B134" r:id="rId76"/>
-    <hyperlink ref="B135" r:id="rId77"/>
-    <hyperlink ref="B136" r:id="rId78"/>
-    <hyperlink ref="B137" r:id="rId79"/>
-    <hyperlink ref="B138" r:id="rId80"/>
-    <hyperlink ref="B139" r:id="rId81"/>
-    <hyperlink ref="B140" r:id="rId82"/>
-    <hyperlink ref="B141" r:id="rId83"/>
-    <hyperlink ref="B142" r:id="rId84"/>
-    <hyperlink ref="B143" r:id="rId85"/>
-    <hyperlink ref="A146" r:id="rId86"/>
-    <hyperlink ref="B147" r:id="rId87" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FVIM%2DVendor%20Invoice%20Management%20Upgrade%20May2021%5FRequester%20Approver%5FJapanese%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM"/>
-    <hyperlink ref="B148" r:id="rId88" display="https://alcon365.sharepoint.com/:p:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B89D9BB48-49C8-4BC1-858C-0C99012AEC46%7D&amp;file=1-4-2.PO%E3%82%AD%E3%83%A3%E3%83%B3%E3%82%BB%E3%83%AB%E3%83%BB%E5%8F%96%E6%B6%88.pptx&amp;action=edit&amp;mobileredirect=true&amp;cid=93fd10e8-d2e3-48d6-8ad0-5cc94dc56304"/>
-    <hyperlink ref="B149" r:id="rId89"/>
-    <hyperlink ref="B158" r:id="rId90"/>
-    <hyperlink ref="B161" r:id="rId91"/>
-    <hyperlink ref="B162" r:id="rId92"/>
-    <hyperlink ref="B168" r:id="rId93"/>
-    <hyperlink ref="B169" r:id="rId94"/>
-    <hyperlink ref="B170" r:id="rId95"/>
-    <hyperlink ref="B171" r:id="rId96"/>
-    <hyperlink ref="B179" r:id="rId97"/>
-    <hyperlink ref="B181" r:id="rId98"/>
-    <hyperlink ref="B5" r:id="rId99"/>
-    <hyperlink ref="B6" r:id="rId100"/>
-    <hyperlink ref="B7" r:id="rId101"/>
-    <hyperlink ref="B23" r:id="rId102"/>
-    <hyperlink ref="B182" r:id="rId103"/>
-    <hyperlink ref="B183" r:id="rId104"/>
-    <hyperlink ref="B184" r:id="rId105" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B887C2330-A6E8-46B5-ACBA-F676866AD2D3%7D&amp;file=SRM%EF%BE%80%EF%BE%9E%EF%BD%B3%EF%BE%9D%EF%BE%8D%EF%BE%9F%EF%BD%B2%EF%BE%92%EF%BE%9D%EF%BE%84%EF%BE%98%EF%BD%B8%EF%BD%B4%EF%BD%BD%EF%BE%84_ver3.xlsx&amp;action=default&amp;mobileredirect=true"/>
-    <hyperlink ref="B185" r:id="rId106"/>
-    <hyperlink ref="B186" r:id="rId107"/>
-    <hyperlink ref="B187" r:id="rId108"/>
-    <hyperlink ref="B188" r:id="rId109"/>
-    <hyperlink ref="B189" r:id="rId110"/>
-    <hyperlink ref="B190" r:id="rId111"/>
-    <hyperlink ref="B191" r:id="rId112"/>
-    <hyperlink ref="B192" r:id="rId113"/>
-    <hyperlink ref="B193" r:id="rId114"/>
-    <hyperlink ref="B194" r:id="rId115"/>
-    <hyperlink ref="B197" r:id="rId116"/>
-    <hyperlink ref="B198" r:id="rId117"/>
-    <hyperlink ref="B199" r:id="rId118"/>
-    <hyperlink ref="B201" r:id="rId119"/>
-    <hyperlink ref="B202" r:id="rId120"/>
-    <hyperlink ref="B203" r:id="rId121"/>
-    <hyperlink ref="B204" r:id="rId122"/>
-    <hyperlink ref="B205" r:id="rId123"/>
-    <hyperlink ref="B206" r:id="rId124"/>
-    <hyperlink ref="B207" r:id="rId125"/>
-    <hyperlink ref="B208" r:id="rId126"/>
-    <hyperlink ref="B209" r:id="rId127"/>
-    <hyperlink ref="B210" r:id="rId128"/>
-    <hyperlink ref="B240" r:id="rId129"/>
-    <hyperlink ref="B241" r:id="rId130"/>
-    <hyperlink ref="B242" r:id="rId131"/>
-    <hyperlink ref="B243" r:id="rId132"/>
-    <hyperlink ref="B246" r:id="rId133" location="a-02"/>
-    <hyperlink ref="B247" r:id="rId134"/>
-    <hyperlink ref="B259" r:id="rId135"/>
-    <hyperlink ref="B264" r:id="rId136" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
-    <hyperlink ref="B265" r:id="rId137" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
-    <hyperlink ref="B266" r:id="rId138" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
-    <hyperlink ref="B267" r:id="rId139" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww"/>
-    <hyperlink ref="B274" r:id="rId140"/>
-    <hyperlink ref="B275" r:id="rId141"/>
-    <hyperlink ref="B276" r:id="rId142"/>
-    <hyperlink ref="B277" r:id="rId143"/>
-    <hyperlink ref="B278" r:id="rId144"/>
-    <hyperlink ref="B280" r:id="rId145"/>
-    <hyperlink ref="B281" r:id="rId146"/>
-    <hyperlink ref="B282" r:id="rId147"/>
-    <hyperlink ref="B283" r:id="rId148"/>
-    <hyperlink ref="B284" r:id="rId149"/>
-    <hyperlink ref="B285" r:id="rId150"/>
-    <hyperlink ref="B286" r:id="rId151"/>
-    <hyperlink ref="B287" r:id="rId152"/>
-    <hyperlink ref="B288" r:id="rId153"/>
-    <hyperlink ref="B289" r:id="rId154"/>
-    <hyperlink ref="B290" r:id="rId155"/>
-    <hyperlink ref="B291" r:id="rId156"/>
-    <hyperlink ref="B292" r:id="rId157"/>
-    <hyperlink ref="B293" r:id="rId158"/>
-    <hyperlink ref="B294" r:id="rId159"/>
-    <hyperlink ref="B295" r:id="rId160"/>
-    <hyperlink ref="B296" r:id="rId161"/>
-    <hyperlink ref="B297" r:id="rId162"/>
-    <hyperlink ref="B298" r:id="rId163"/>
-    <hyperlink ref="B299" r:id="rId164"/>
-    <hyperlink ref="B300" r:id="rId165"/>
-    <hyperlink ref="B301" r:id="rId166"/>
-    <hyperlink ref="B302" r:id="rId167"/>
-    <hyperlink ref="B303" r:id="rId168" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2F%E3%82%B0%E3%83%AD%E3%83%BC%E3%83%90%E3%83%AB%E7%89%88%E3%80%80%E3%82%A8%E3%83%B3%E3%83%89%E3%83%A6%E3%83%BC%E3%82%B6%E3%83%BCFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
-    <hyperlink ref="B304" r:id="rId169" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%5FEnd%5FUser%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
-    <hyperlink ref="B305" r:id="rId170" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FJA%5FGlobal%20TE%20policy%5FFAQ%2DR%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs"/>
-    <hyperlink ref="B306" r:id="rId171" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FGlobal%20TE%20policy%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs"/>
-    <hyperlink ref="B307" r:id="rId172" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%E3%83%A2%E3%83%90%E3%82%A4%E3%83%AB%E3%82%A2%E3%83%97%E3%83%AA%E3%83%87%E3%83%A2%2Ewebex&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides&amp;p=14"/>
-    <hyperlink ref="B308" r:id="rId173"/>
-    <hyperlink ref="B309" r:id="rId174"/>
-    <hyperlink ref="B310" r:id="rId175"/>
-    <hyperlink ref="B311" r:id="rId176"/>
-    <hyperlink ref="B312" r:id="rId177"/>
-    <hyperlink ref="B313" r:id="rId178"/>
-    <hyperlink ref="B314" r:id="rId179"/>
-    <hyperlink ref="B315" r:id="rId180"/>
-    <hyperlink ref="B316" r:id="rId181"/>
-    <hyperlink ref="B317" r:id="rId182"/>
-    <hyperlink ref="B318" r:id="rId183"/>
-    <hyperlink ref="B319" r:id="rId184"/>
-    <hyperlink ref="B320" r:id="rId185"/>
-    <hyperlink ref="B321" r:id="rId186"/>
-    <hyperlink ref="B322" r:id="rId187"/>
-    <hyperlink ref="B323" r:id="rId188"/>
-    <hyperlink ref="B324" r:id="rId189"/>
-    <hyperlink ref="B325" r:id="rId190"/>
-    <hyperlink ref="B326" r:id="rId191"/>
-    <hyperlink ref="B327" r:id="rId192"/>
-    <hyperlink ref="B328" r:id="rId193"/>
-    <hyperlink ref="B329" r:id="rId194"/>
-    <hyperlink ref="B330" r:id="rId195"/>
-    <hyperlink ref="B331" r:id="rId196"/>
-    <hyperlink ref="B332" r:id="rId197"/>
-    <hyperlink ref="B333" r:id="rId198"/>
-    <hyperlink ref="B334" r:id="rId199"/>
-    <hyperlink ref="B335" r:id="rId200"/>
-    <hyperlink ref="B336" r:id="rId201"/>
-    <hyperlink ref="B338" r:id="rId202"/>
-    <hyperlink ref="B339" r:id="rId203" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1"/>
-    <hyperlink ref="B340" r:id="rId204"/>
-    <hyperlink ref="B343" r:id="rId205"/>
-    <hyperlink ref="B344" r:id="rId206"/>
-    <hyperlink ref="B345" r:id="rId207"/>
-    <hyperlink ref="B346" r:id="rId208"/>
-    <hyperlink ref="B347" r:id="rId209"/>
-    <hyperlink ref="B348" r:id="rId210"/>
-    <hyperlink ref="B349" r:id="rId211"/>
-    <hyperlink ref="B350" r:id="rId212"/>
-    <hyperlink ref="B351" r:id="rId213"/>
-    <hyperlink ref="B352" r:id="rId214"/>
-    <hyperlink ref="B353" r:id="rId215"/>
-    <hyperlink ref="B355" r:id="rId216"/>
-    <hyperlink ref="B356" r:id="rId217"/>
-    <hyperlink ref="B357" r:id="rId218"/>
-    <hyperlink ref="B358" r:id="rId219"/>
-    <hyperlink ref="B359" r:id="rId220"/>
-    <hyperlink ref="B360" r:id="rId221"/>
-    <hyperlink ref="B361" r:id="rId222"/>
-    <hyperlink ref="B362" r:id="rId223"/>
-    <hyperlink ref="B363" r:id="rId224"/>
-    <hyperlink ref="B364" r:id="rId225"/>
-    <hyperlink ref="B365" r:id="rId226"/>
-    <hyperlink ref="B366" r:id="rId227"/>
-    <hyperlink ref="B367" r:id="rId228"/>
-    <hyperlink ref="B368" r:id="rId229"/>
-    <hyperlink ref="B369" r:id="rId230"/>
-    <hyperlink ref="B370:B371" r:id="rId231" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\Withholding Tax\PSCへ提出_1110払源泉税.msg"/>
-    <hyperlink ref="B372" r:id="rId232"/>
-    <hyperlink ref="B373" r:id="rId233"/>
-    <hyperlink ref="B374" r:id="rId234"/>
-    <hyperlink ref="B375" r:id="rId235"/>
-    <hyperlink ref="B376" r:id="rId236"/>
-    <hyperlink ref="B377" r:id="rId237"/>
-    <hyperlink ref="B378" r:id="rId238"/>
-    <hyperlink ref="B379" r:id="rId239"/>
-    <hyperlink ref="B380" r:id="rId240"/>
-    <hyperlink ref="B381" r:id="rId241"/>
-    <hyperlink ref="B383" r:id="rId242"/>
-    <hyperlink ref="B384" r:id="rId243"/>
-    <hyperlink ref="B385" r:id="rId244"/>
-    <hyperlink ref="B386" r:id="rId245"/>
-    <hyperlink ref="B387" r:id="rId246"/>
-    <hyperlink ref="B388" r:id="rId247"/>
-    <hyperlink ref="B58" r:id="rId248"/>
-    <hyperlink ref="B57" r:id="rId249"/>
-    <hyperlink ref="B395" r:id="rId250"/>
-    <hyperlink ref="B396" r:id="rId251"/>
-    <hyperlink ref="B397" r:id="rId252"/>
-    <hyperlink ref="B398" r:id="rId253"/>
-    <hyperlink ref="B399" r:id="rId254"/>
-    <hyperlink ref="B400" r:id="rId255"/>
-    <hyperlink ref="B401" r:id="rId256"/>
-    <hyperlink ref="B402" r:id="rId257"/>
-    <hyperlink ref="B403" r:id="rId258"/>
-    <hyperlink ref="B405" r:id="rId259"/>
-    <hyperlink ref="B406" r:id="rId260"/>
-    <hyperlink ref="B407" r:id="rId261"/>
-    <hyperlink ref="B408" r:id="rId262"/>
-    <hyperlink ref="B409" r:id="rId263"/>
-    <hyperlink ref="B410" r:id="rId264"/>
-    <hyperlink ref="B411" r:id="rId265"/>
-    <hyperlink ref="B412" r:id="rId266"/>
-    <hyperlink ref="B413" r:id="rId267"/>
-    <hyperlink ref="B414" r:id="rId268"/>
-    <hyperlink ref="B415" r:id="rId269"/>
-    <hyperlink ref="B416" r:id="rId270"/>
-    <hyperlink ref="B417" r:id="rId271"/>
-    <hyperlink ref="B418" r:id="rId272"/>
-    <hyperlink ref="B419" r:id="rId273"/>
-    <hyperlink ref="B421" r:id="rId274"/>
-    <hyperlink ref="B429" r:id="rId275"/>
-    <hyperlink ref="B430" r:id="rId276"/>
-    <hyperlink ref="B431" r:id="rId277"/>
-    <hyperlink ref="B432" r:id="rId278"/>
-    <hyperlink ref="B433" r:id="rId279"/>
-    <hyperlink ref="B436" r:id="rId280" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday"/>
-    <hyperlink ref="B437" r:id="rId281" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday"/>
-    <hyperlink ref="B438" r:id="rId282" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday"/>
-    <hyperlink ref="B439" r:id="rId283"/>
-    <hyperlink ref="B441" r:id="rId284"/>
-    <hyperlink ref="B442" r:id="rId285"/>
-    <hyperlink ref="B443" r:id="rId286"/>
-    <hyperlink ref="B444" r:id="rId287"/>
-    <hyperlink ref="B445" r:id="rId288"/>
-    <hyperlink ref="B446" r:id="rId289"/>
-    <hyperlink ref="B447" r:id="rId290"/>
-    <hyperlink ref="B448" r:id="rId291"/>
-    <hyperlink ref="B449" r:id="rId292"/>
-    <hyperlink ref="B450" r:id="rId293"/>
-    <hyperlink ref="B451" r:id="rId294"/>
-    <hyperlink ref="B452" r:id="rId295"/>
-    <hyperlink ref="B453" r:id="rId296"/>
-    <hyperlink ref="B454" r:id="rId297"/>
-    <hyperlink ref="B455" r:id="rId298"/>
-    <hyperlink ref="B456" r:id="rId299"/>
-    <hyperlink ref="B457" r:id="rId300"/>
-    <hyperlink ref="B458" r:id="rId301"/>
-    <hyperlink ref="B459" r:id="rId302" display="https://mdg.alcon.net/nwbc/?sap-client=010&amp;sap-language=EN&amp;sap-nwbc-context=03HM333035D633D53336000128D3C800C2350EF03304320D416C20C32DA3A4A4A0D84A5F3F37255D2F3127393F4F2F2FB5C4CAD2C0DC403FAF3C2959DFBE38B1403739273335AFC416A8410DC4CD49CC4B2F4D4C4FB575F50300&amp;sap-theme=sap_corbu&amp;sap-nwbc-node=0000000102"/>
-    <hyperlink ref="B460" r:id="rId303" display="https://grc.alcon.net/nwbc/?sap-nwbc-node=0000000005&amp;sap-nwbc-context=03HM333035D633D33336748AB232700E700F7274D675720C760D0D760D8A77F7718A3730307434303433802833303230360001E380101320D310C80400&amp;sap-client=010&amp;sap-language=JA&amp;sap-nwbc-history_item=&amp;sap-theme=sap_corbu"/>
-    <hyperlink ref="B461" r:id="rId304" location="ZMYBANK-display"/>
-    <hyperlink ref="B462" r:id="rId305"/>
-    <hyperlink ref="B463" r:id="rId306"/>
-    <hyperlink ref="B464" r:id="rId307"/>
-    <hyperlink ref="B465" r:id="rId308" display="maiko.okamoto@alcon.com"/>
-    <hyperlink ref="B467" r:id="rId309" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%20Table%20change%20request%20form%E8%A6%8B%E6%9C%AC%5F2021Nov%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM"/>
-    <hyperlink ref="B468" r:id="rId310" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%5FTable%5FMaintence%5FRequest%5FForm%20%28002%29%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM"/>
-    <hyperlink ref="B469" r:id="rId311"/>
-    <hyperlink ref="B471" r:id="rId312"/>
-    <hyperlink ref="B473" r:id="rId313"/>
-    <hyperlink ref="B474" r:id="rId314"/>
-    <hyperlink ref="B475" r:id="rId315"/>
-    <hyperlink ref="B476" r:id="rId316"/>
-    <hyperlink ref="B477" r:id="rId317" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides"/>
-    <hyperlink ref="B478" r:id="rId318" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents"/>
-    <hyperlink ref="B479" r:id="rId319" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents"/>
-    <hyperlink ref="B480" r:id="rId320"/>
-    <hyperlink ref="B484" r:id="rId321"/>
-    <hyperlink ref="B485" r:id="rId322"/>
-    <hyperlink ref="B486" r:id="rId323"/>
-    <hyperlink ref="B487" r:id="rId324" location="/site/FRAGlobal/workbooks/8033/views"/>
-    <hyperlink ref="B488" r:id="rId325" location="/site/FRAGlobal/workbooks/8033/views"/>
-    <hyperlink ref="B489" r:id="rId326"/>
-    <hyperlink ref="B490" r:id="rId327"/>
-    <hyperlink ref="B491" r:id="rId328"/>
-    <hyperlink ref="B492" r:id="rId329"/>
-    <hyperlink ref="B493" r:id="rId330"/>
-    <hyperlink ref="B494" r:id="rId331"/>
-    <hyperlink ref="B498" r:id="rId332"/>
-    <hyperlink ref="B500" r:id="rId333"/>
-    <hyperlink ref="B501" r:id="rId334"/>
-    <hyperlink ref="B506" r:id="rId335"/>
-    <hyperlink ref="B519" r:id="rId336"/>
-    <hyperlink ref="B521" r:id="rId337"/>
-    <hyperlink ref="B522" r:id="rId338"/>
-    <hyperlink ref="B523" r:id="rId339"/>
-    <hyperlink ref="B525" r:id="rId340" display="http://alusfw-sp353107.alcon.net/NimbusFinance/CtrlWebISAPI.dll/app/diagram/0:9B906E1EB57A44FB8CF3F2821EA071DE"/>
-    <hyperlink ref="B526" r:id="rId341"/>
-    <hyperlink ref="B539" r:id="rId342"/>
-    <hyperlink ref="B540" r:id="rId343"/>
-    <hyperlink ref="B541" r:id="rId344"/>
-    <hyperlink ref="B543" r:id="rId345"/>
-    <hyperlink ref="B542" r:id="rId346"/>
-    <hyperlink ref="B544" r:id="rId347"/>
-    <hyperlink ref="B546" r:id="rId348"/>
-    <hyperlink ref="B547" r:id="rId349"/>
-    <hyperlink ref="B550" r:id="rId350"/>
-    <hyperlink ref="B551" r:id="rId351"/>
-    <hyperlink ref="B552" r:id="rId352"/>
-    <hyperlink ref="B553" r:id="rId353"/>
-    <hyperlink ref="B554" r:id="rId354"/>
-    <hyperlink ref="B555" r:id="rId355"/>
-    <hyperlink ref="B556" r:id="rId356"/>
-    <hyperlink ref="B557" r:id="rId357"/>
-    <hyperlink ref="B558" r:id="rId358"/>
-    <hyperlink ref="B559" r:id="rId359"/>
-    <hyperlink ref="B560" r:id="rId360"/>
-    <hyperlink ref="B561" r:id="rId361"/>
-    <hyperlink ref="B562" r:id="rId362"/>
-    <hyperlink ref="B563" r:id="rId363"/>
-    <hyperlink ref="B564" r:id="rId364"/>
-    <hyperlink ref="B565" r:id="rId365"/>
-    <hyperlink ref="B566" r:id="rId366"/>
-    <hyperlink ref="B567" r:id="rId367" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\SAP\Attached invoice_FBL1N.mp4"/>
-    <hyperlink ref="B568" r:id="rId368" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\SAP\Attached invoice_FBL1N.mp4"/>
-    <hyperlink ref="B549" r:id="rId369" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FNew%20Global%20Travel%20%20Expense%20Policy%5FEffective%20August%201%202020%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents"/>
-    <hyperlink ref="B572" r:id="rId370"/>
-    <hyperlink ref="B573" r:id="rId371"/>
-    <hyperlink ref="B574" r:id="rId372"/>
-    <hyperlink ref="B575" r:id="rId373"/>
-    <hyperlink ref="B576" r:id="rId374"/>
-    <hyperlink ref="B577" r:id="rId375"/>
-    <hyperlink ref="B578" r:id="rId376"/>
-    <hyperlink ref="B579" r:id="rId377"/>
-    <hyperlink ref="B583" r:id="rId378"/>
-    <hyperlink ref="B66" r:id="rId379"/>
-    <hyperlink ref="B606" r:id="rId380"/>
-    <hyperlink ref="B607" r:id="rId381"/>
-    <hyperlink ref="B608" r:id="rId382" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top+Resources%2FJapanHR_CompanyHousing%2F%EF%BC%9CALJ%EF%BC%9E%E7%A4%BE%E5%AE%85%E3%83%BB%E9%A7%90%E8%BB%8A%E5%A0%B4%E3%81%AE%E3%82%AC%E3%82%A4%E3%83%89%E3%83%96%E3%83%83%E3%82%AF_20210414.pdf&amp;parent=%2Fsites%2FInSight%2F263Top+Resources%2FJapanHR_CompanyHousing&amp;isSPOFile=1&amp;OR=Teams-HL&amp;CT=1643358574668&amp;sourceId=&amp;params=%7B%22AppName%22%3A%22Teams-Desktop%22%2C%22AppVersion%22%3A%2227%2F21110108720%22%7D"/>
-    <hyperlink ref="B609" r:id="rId383"/>
-    <hyperlink ref="B610" r:id="rId384"/>
-    <hyperlink ref="B611" r:id="rId385"/>
-    <hyperlink ref="B612" r:id="rId386"/>
-    <hyperlink ref="B613" r:id="rId387"/>
-    <hyperlink ref="B614" r:id="rId388"/>
-    <hyperlink ref="B615" r:id="rId389"/>
-    <hyperlink ref="B616" r:id="rId390"/>
-    <hyperlink ref="B617" r:id="rId391"/>
-    <hyperlink ref="B618" r:id="rId392"/>
-    <hyperlink ref="B619" r:id="rId393"/>
-    <hyperlink ref="B620" r:id="rId394"/>
-    <hyperlink ref="B621" r:id="rId395"/>
-    <hyperlink ref="B645" r:id="rId396" display="https://nam12.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.linkedin.com%2Flearning%2Fexcel-essential-training-office-365-microsoft-365%3FcontextUrn%3Durn%253Ali%253AlyndaLearningPath%253A5bc7873e498ed19914588530%26u%3D2154545&amp;data=04%7C01%7CHanis.Jaffar%40alcon.com%7Cbbe859168c264f9b385308d9e779c269%7C34cd94b5d86c447f8d9b81b4ff94d329%7C0%7C0%7C637795332408739455%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000&amp;sdata=UhnPLkJkhVfQ7DsuV1C4Refe45XwAj2HS0fNTkkdPds%3D&amp;reserved=0"/>
-    <hyperlink ref="B646" r:id="rId397" display="https://nam12.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.linkedin.com%2Flearning%2Fexcel-pivottables-for-beginners%3FcontextUrn%3Durn%253Ali%253AlyndaLearningPath%253A5bc7873e498ed19914588530%26u%3D2154545&amp;data=04%7C01%7CHanis.Jaffar%40alcon.com%7Cbbe859168c264f9b385308d9e779c269%7C34cd94b5d86c447f8d9b81b4ff94d329%7C0%7C0%7C637795332408739455%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000&amp;sdata=C5bHVDyRfQOXhO%2FZD7XCf4YpTH3VLbLvLcXE3Yz1%2Bv0%3D&amp;reserved=0"/>
-    <hyperlink ref="B647" r:id="rId398" display="https://nam12.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.linkedin.com%2Flearning%2Fexcel-introduction-to-formulas-and-functions%3FcontextUrn%3Durn%253Ali%253AlyndaLearningPath%253A5bc7873e498ed19914588530%26u%3D2154545&amp;data=04%7C01%7CHanis.Jaffar%40alcon.com%7Cbbe859168c264f9b385308d9e779c269%7C34cd94b5d86c447f8d9b81b4ff94d329%7C0%7C0%7C637795332408739455%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000&amp;sdata=Iprb6IxgarShNz%2BbY4eV8OwgnxVO1ILXzmeKPDS3eEw%3D&amp;reserved=0"/>
-    <hyperlink ref="B651" r:id="rId399" display="Newjoiner and resigner's expense"/>
-    <hyperlink ref="B652" r:id="rId400"/>
-    <hyperlink ref="B655" r:id="rId401"/>
-    <hyperlink ref="B656" r:id="rId402"/>
-    <hyperlink ref="B657" r:id="rId403"/>
-    <hyperlink ref="B658" r:id="rId404"/>
-    <hyperlink ref="B660" r:id="rId405"/>
-    <hyperlink ref="B661" r:id="rId406"/>
-    <hyperlink ref="B662" r:id="rId407"/>
-    <hyperlink ref="B663" r:id="rId408"/>
-    <hyperlink ref="B664" r:id="rId409"/>
-    <hyperlink ref="B665" r:id="rId410"/>
-    <hyperlink ref="B667" r:id="rId411"/>
-    <hyperlink ref="B668" r:id="rId412"/>
-    <hyperlink ref="B669" r:id="rId413"/>
-    <hyperlink ref="B670" r:id="rId414"/>
-    <hyperlink ref="B671" r:id="rId415"/>
-    <hyperlink ref="B672" r:id="rId416"/>
-    <hyperlink ref="B673" r:id="rId417"/>
-    <hyperlink ref="B674" r:id="rId418"/>
-    <hyperlink ref="B666" r:id="rId419"/>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B24" display="https://alcon365.sharepoint.com/sites/alconfra/SitePages/MasterData.aspx?RootFolder=%2Fsites%2Falconfra%2FFinance%20Master%20Data%20Management%2FApproval%20Table%20Maintenance&amp;FolderCTID=0x012000F818F3CCE22AE94C86C3A970A6E10830&amp;View=%7B785A14CF-1D11-4535-" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B22" r:id="rId4" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId13" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FNew%20Global%20Travel%20%20Expense%20Policy%5FEffective%20August%201%202020%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B28" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B29" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B30" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B36" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B37" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B38" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B39" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B40" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B41" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B42" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B44" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B45" r:id="rId29" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B46" r:id="rId30" display="I:\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JAPAN\04 R2P MIGRATION\1  RECORDING AP MIGRATION FEB TO MAR 2021" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B61" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B62" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B63" r:id="rId33" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2F%E7%B5%8C%E8%B2%BB%E7%B2%BE%E7%AE%97%E3%81%8A%E7%9F%A5%E3%82%89%E3%81%9B%E3%81%AE%E6%89%8B%E9%A0%86%E6%9B%B8%20V2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B65" r:id="rId34" display="https://alcon365.sharepoint.com/sites/InSight/096DocLib2/Forms/TheLensNameTitlePage.aspx?viewid=4a09b348%2D50df%2D46b7%2Da194%2D518047515835&amp;id=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations%2FTheLensPolicy%5Fen%2DEN%2Epdf&amp;parent=%2Fsites%2FInSight%2F096DocLib2%2FTheLensTranslations" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B67" r:id="rId35" display="https://alcon365.sharepoint.com/sites/InSight/230DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG%2FHCP%E3%81%B8%E3%81%AE%E9%A3%B2%E9%A3%9F%E3%83%BB%E6%97%85%E8%B2%BB%E7%AD%89%E3%81%AE%E6%8F%90%E4%BE%9B%E4%B8%80%E8%A6%A7-%20%2020200801_final.pdf&amp;parent=%2Fsites%2FInSight%2F230DocLib%2F%E3%80%90%E5%85%B1%E9%80%9A%E3%80%91SOP%E3%83%BBQRG" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B68" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B69" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B70" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B71" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B72" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B73" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B99" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B100" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B101" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B102" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B103" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B104" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B105" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B106" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B107" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B108" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B109" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B111" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B112" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B114" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B115" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B116" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B117" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B118" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B119" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B120" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B121" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B122" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FAlcon%20Japan%20How%20to%20use%20expense%5F202101%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVI" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B113" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B123" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B124" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B125" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B126" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B127" r:id="rId68" display="https://alcon365.sharepoint.com/sites/InSight/SitePages/230/%E7%B2%BE%E7%AE%97%E3%81%A8%E9%80%8F%E6%98%8E%E6%80%A7%E3%82%AC%E3%82%A4%E3%83%89%E3%83%A9%E3%82%A4%E3%83%B3.aspx" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B128" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B110" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B129" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B130" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B131" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B132" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B133" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B134" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B135" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B136" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B137" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B138" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B139" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B140" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B141" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B142" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B143" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A146" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B147" r:id="rId87" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FVIM%2DVendor%20Invoice%20Management%20Upgrade%20May2021%5FRequester%20Approver%5FJapanese%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B148" r:id="rId88" display="https://alcon365.sharepoint.com/:p:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B89D9BB48-49C8-4BC1-858C-0C99012AEC46%7D&amp;file=1-4-2.PO%E3%82%AD%E3%83%A3%E3%83%B3%E3%82%BB%E3%83%AB%E3%83%BB%E5%8F%96%E6%B6%88.pptx&amp;action=edit&amp;mobileredirect=true&amp;cid=93fd10e8-d2e3-48d6-8ad0-5cc94dc56304" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B149" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B158" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B161" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B162" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B168" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B169" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B170" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B171" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B179" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B181" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B5" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B6" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B7" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B23" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B182" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B183" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B184" r:id="rId105" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7B887C2330-A6E8-46B5-ACBA-F676866AD2D3%7D&amp;file=SRM%EF%BE%80%EF%BE%9E%EF%BD%B3%EF%BE%9D%EF%BE%8D%EF%BE%9F%EF%BD%B2%EF%BE%92%EF%BE%9D%EF%BE%84%EF%BE%98%EF%BD%B8%EF%BD%B4%EF%BD%BD%EF%BE%84_ver3.xlsx&amp;action=default&amp;mobileredirect=true" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B185" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B186" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B187" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B188" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B189" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B190" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B191" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B192" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B193" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B194" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B197" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B198" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B199" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B201" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B202" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B203" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B204" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B205" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B206" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B207" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B208" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B209" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B210" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B240" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B241" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B242" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B243" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B246" r:id="rId133" location="a-02" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B247" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B259" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B264" r:id="rId136" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B265" r:id="rId137" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B266" r:id="rId138" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B267" r:id="rId139" tooltip="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6.%20AGS%20%E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" display="https://alcon365.sharepoint.com/:b:/r/sites/InSight/282DocLib/SRM%E3%83%BBSIM/SRM/6. AGS %E3%83%9E%E3%83%8B%E3%83%A5%E3%82%A2%E3%83%AB/2-1_GR%E3%81%A8%E5%8F%96%E6%B6%88.pdf?csf=1&amp;web=1&amp;e=0ukLww" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B274" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B275" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B276" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B277" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B278" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B280" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B281" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B282" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B283" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B284" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B285" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B286" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="B287" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B288" r:id="rId153" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="B289" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B290" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="B291" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B292" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="B293" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B294" r:id="rId159" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="B295" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B296" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B297" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B298" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="B299" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B300" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B301" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B302" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="B303" r:id="rId168" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2F%E3%82%B0%E3%83%AD%E3%83%BC%E3%83%90%E3%83%AB%E7%89%88%E3%80%80%E3%82%A8%E3%83%B3%E3%83%89%E3%83%A6%E3%83%BC%E3%82%B6%E3%83%BCFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B304" r:id="rId169" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%5FEnd%5FUser%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B305" r:id="rId170" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FJA%5FGlobal%20TE%20policy%5FFAQ%2DR%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B306" r:id="rId171" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs%2FGlobal%20TE%20policy%5FFAQ%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F5%5FContacts%20%26%20FAQs" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="B307" r:id="rId172" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FConcur%E3%83%A2%E3%83%90%E3%82%A4%E3%83%AB%E3%82%A2%E3%83%97%E3%83%AA%E3%83%87%E3%83%A2%2Ewebex&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides&amp;p=14" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="B308" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="B309" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="B310" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="B311" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="B312" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="B313" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="B314" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="B315" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="B316" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="B317" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="B318" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="B319" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="B320" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="B321" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="B322" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="B323" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="B324" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="B325" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="B326" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="B327" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="B328" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="B329" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="B330" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="B331" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="B332" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="B333" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="B334" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="B335" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="B336" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="B338" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="B339" r:id="rId203" display="https://alcon365.sharepoint.com/:x:/r/sites/InSight/_layouts/15/Doc.aspx?sourcedoc=%7BFACE8369-FF19-4663-B67B-F3542DD1F9C4%7D&amp;file=Japan_%E6%96%B0%E6%97%A7ACC-GL%20Mapping%E5%AF%BE%E6%AF%94%E8%A1%A8_%E3%82%A4%E3%83%B3%E3%83%88%E3%83%A9%E6%8E%B2%E8%BC%89%E7%94%A8.xlsx&amp;action=default&amp;mobileredirect=true&amp;DefaultItemOpen=1" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="B340" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="B343" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="B344" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="B345" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="B346" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="B347" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="B348" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="B349" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="B350" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="B351" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="B352" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="B353" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="B355" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="B356" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="B357" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="B358" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="B359" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="B360" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="B361" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="B362" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="B363" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="B364" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="B365" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="B366" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="B367" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="B368" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="B369" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="B370:B371" r:id="rId231" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\Withholding Tax\PSCへ提出_1110払源泉税.msg" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="B372" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="B373" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="B374" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="B375" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="B376" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="B377" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="B378" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="B379" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="B380" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="B381" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="B383" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="B384" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="B385" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="B386" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="B387" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="B388" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="B58" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="B57" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="B395" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="B396" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="B397" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="B398" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="B399" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="B400" r:id="rId255" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="B401" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="B402" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="B403" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="B405" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="B406" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="B407" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="B408" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="B409" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="B410" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="B411" r:id="rId265" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="B412" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="B413" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="B414" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="B415" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="B416" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="B417" r:id="rId271" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="B418" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="B419" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="B421" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="B429" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="B430" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="B431" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="B432" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="B433" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="B436" r:id="rId280" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="B437" r:id="rId281" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="B438" r:id="rId282" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday%2FAssociate%20Directory%2Ev2%5F20210916%2Epdf&amp;parent=%2Fsites%2FInSight%2F263Top%20Resources%2FJapanHR%5FWorkday" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="B439" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="B441" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="B442" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="B443" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="B444" r:id="rId287" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="B445" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="B446" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="B447" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="B448" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="B449" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="B450" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="B451" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="B452" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="B453" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="B454" r:id="rId297" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="B455" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="B456" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="B457" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="B458" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="B459" r:id="rId302" display="https://mdg.alcon.net/nwbc/?sap-client=010&amp;sap-language=EN&amp;sap-nwbc-context=03HM333035D633D53336000128D3C800C2350EF03304320D416C20C32DA3A4A4A0D84A5F3F37255D2F3127393F4F2F2FB5C4CAD2C0DC403FAF3C2959DFBE38B1403739273335AFC416A8410DC4CD49CC4B2F4D4C4FB575F50300&amp;sap-theme=sap_corbu&amp;sap-nwbc-node=0000000102" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="B460" r:id="rId303" display="https://grc.alcon.net/nwbc/?sap-nwbc-node=0000000005&amp;sap-nwbc-context=03HM333035D633D33336748AB232700E700F7274D675720C760D0D760D8A77F7718A3730307434303433802833303230360001E380101320D310C80400&amp;sap-client=010&amp;sap-language=JA&amp;sap-nwbc-history_item=&amp;sap-theme=sap_corbu" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="B461" r:id="rId304" location="ZMYBANK-display" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="B462" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="B463" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="B464" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="B465" r:id="rId308" display="maiko.okamoto@alcon.com" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="B467" r:id="rId309" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%20Table%20change%20request%20form%E8%A6%8B%E6%9C%AC%5F2021Nov%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="B468" r:id="rId310" display="https://alcon365.sharepoint.com/sites/InSight/239Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM%2FApproval%5FTable%5FMaintence%5FRequest%5FForm%20%28002%29%2Epdf&amp;parent=%2Fsites%2FInSight%2F239Top%20Resources%2FR2P%2FVIM" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="B469" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="B471" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="B473" r:id="rId313" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="B474" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="B475" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="B476" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="B477" r:id="rId317" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides%2FEN%5FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%5F202105%2Epdf%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F2%5FHow%2DTo%20Guides" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="B478" r:id="rId318" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="B479" r:id="rId319" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FGlobal%5FEnd%5FUser%20Training%20%2D%20All%20employees%2DR2%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="B480" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="B484" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="B485" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="B486" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="B487" r:id="rId324" location="/site/FRAGlobal/workbooks/8033/views" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
+    <hyperlink ref="B488" r:id="rId325" location="/site/FRAGlobal/workbooks/8033/views" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
+    <hyperlink ref="B489" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
+    <hyperlink ref="B490" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
+    <hyperlink ref="B491" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="B492" r:id="rId329" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
+    <hyperlink ref="B493" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
+    <hyperlink ref="B494" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
+    <hyperlink ref="B498" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
+    <hyperlink ref="B500" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
+    <hyperlink ref="B501" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
+    <hyperlink ref="B506" r:id="rId335" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
+    <hyperlink ref="B519" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
+    <hyperlink ref="B521" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
+    <hyperlink ref="B522" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
+    <hyperlink ref="B523" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
+    <hyperlink ref="B525" r:id="rId340" display="http://alusfw-sp353107.alcon.net/NimbusFinance/CtrlWebISAPI.dll/app/diagram/0:9B906E1EB57A44FB8CF3F2821EA071DE" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
+    <hyperlink ref="B526" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
+    <hyperlink ref="B539" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
+    <hyperlink ref="B540" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
+    <hyperlink ref="B541" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
+    <hyperlink ref="B543" r:id="rId345" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
+    <hyperlink ref="B542" r:id="rId346" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
+    <hyperlink ref="B544" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
+    <hyperlink ref="B546" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
+    <hyperlink ref="B547" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
+    <hyperlink ref="B550" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
+    <hyperlink ref="B551" r:id="rId351" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
+    <hyperlink ref="B552" r:id="rId352" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
+    <hyperlink ref="B553" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
+    <hyperlink ref="B554" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
+    <hyperlink ref="B555" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
+    <hyperlink ref="B556" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
+    <hyperlink ref="B557" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
+    <hyperlink ref="B558" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
+    <hyperlink ref="B559" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
+    <hyperlink ref="B560" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
+    <hyperlink ref="B561" r:id="rId361" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
+    <hyperlink ref="B562" r:id="rId362" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
+    <hyperlink ref="B563" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
+    <hyperlink ref="B564" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
+    <hyperlink ref="B565" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
+    <hyperlink ref="B566" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
+    <hyperlink ref="B567" r:id="rId367" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\SAP\Attached invoice_FBL1N.mp4" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
+    <hyperlink ref="B568" r:id="rId368" display="\\Alcon.net\jphq-dfs\DATA\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\Asano\SAP\Attached invoice_FBL1N.mp4" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
+    <hyperlink ref="B549" r:id="rId369" display="https://alcon365.sharepoint.com/sites/InSight/289DocLib/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents%2FNew%20Global%20Travel%20%20Expense%20Policy%5FEffective%20August%201%202020%2Epdf&amp;parent=%2Fsites%2FInSight%2F289DocLib%2FFRA%20Operations%2FGPO%2FT%26E%2FT%26E%20JAPAN%2F1%5FGeneral%20Documents" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
+    <hyperlink ref="B572" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
+    <hyperlink ref="B573" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
+    <hyperlink ref="B574" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
+    <hyperlink ref="B575" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
+    <hyperlink ref="B576" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
+    <hyperlink ref="B577" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
+    <hyperlink ref="B578" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
+    <hyperlink ref="B579" r:id="rId377" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
+    <hyperlink ref="B583" r:id="rId378" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
+    <hyperlink ref="B66" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
+    <hyperlink ref="B606" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
+    <hyperlink ref="B607" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
+    <hyperlink ref="B608" r:id="rId382" display="https://alcon365.sharepoint.com/sites/InSight/263Top%20Resources/Forms/AllItems.aspx?id=%2Fsites%2FInSight%2F263Top+Resources%2FJapanHR_CompanyHousing%2F%EF%BC%9CALJ%EF%BC%9E%E7%A4%BE%E5%AE%85%E3%83%BB%E9%A7%90%E8%BB%8A%E5%A0%B4%E3%81%AE%E3%82%AC%E3%82%A4%E3%83%89%E3%83%96%E3%83%83%E3%82%AF_20210414.pdf&amp;parent=%2Fsites%2FInSight%2F263Top+Resources%2FJapanHR_CompanyHousing&amp;isSPOFile=1&amp;OR=Teams-HL&amp;CT=1643358574668&amp;sourceId=&amp;params=%7B%22AppName%22%3A%22Teams-Desktop%22%2C%22AppVersion%22%3A%2227%2F21110108720%22%7D" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
+    <hyperlink ref="B609" r:id="rId383" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
+    <hyperlink ref="B610" r:id="rId384" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
+    <hyperlink ref="B611" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
+    <hyperlink ref="B612" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
+    <hyperlink ref="B613" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
+    <hyperlink ref="B614" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
+    <hyperlink ref="B615" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
+    <hyperlink ref="B616" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
+    <hyperlink ref="B617" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
+    <hyperlink ref="B618" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
+    <hyperlink ref="B619" r:id="rId393" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
+    <hyperlink ref="B620" r:id="rId394" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
+    <hyperlink ref="B621" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
+    <hyperlink ref="B645" r:id="rId396" display="https://nam12.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.linkedin.com%2Flearning%2Fexcel-essential-training-office-365-microsoft-365%3FcontextUrn%3Durn%253Ali%253AlyndaLearningPath%253A5bc7873e498ed19914588530%26u%3D2154545&amp;data=04%7C01%7CHanis.Jaffar%40alcon.com%7Cbbe859168c264f9b385308d9e779c269%7C34cd94b5d86c447f8d9b81b4ff94d329%7C0%7C0%7C637795332408739455%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000&amp;sdata=UhnPLkJkhVfQ7DsuV1C4Refe45XwAj2HS0fNTkkdPds%3D&amp;reserved=0" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
+    <hyperlink ref="B646" r:id="rId397" display="https://nam12.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.linkedin.com%2Flearning%2Fexcel-pivottables-for-beginners%3FcontextUrn%3Durn%253Ali%253AlyndaLearningPath%253A5bc7873e498ed19914588530%26u%3D2154545&amp;data=04%7C01%7CHanis.Jaffar%40alcon.com%7Cbbe859168c264f9b385308d9e779c269%7C34cd94b5d86c447f8d9b81b4ff94d329%7C0%7C0%7C637795332408739455%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000&amp;sdata=C5bHVDyRfQOXhO%2FZD7XCf4YpTH3VLbLvLcXE3Yz1%2Bv0%3D&amp;reserved=0" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
+    <hyperlink ref="B647" r:id="rId398" display="https://nam12.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.linkedin.com%2Flearning%2Fexcel-introduction-to-formulas-and-functions%3FcontextUrn%3Durn%253Ali%253AlyndaLearningPath%253A5bc7873e498ed19914588530%26u%3D2154545&amp;data=04%7C01%7CHanis.Jaffar%40alcon.com%7Cbbe859168c264f9b385308d9e779c269%7C34cd94b5d86c447f8d9b81b4ff94d329%7C0%7C0%7C637795332408739455%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C3000&amp;sdata=Iprb6IxgarShNz%2BbY4eV8OwgnxVO1ILXzmeKPDS3eEw%3D&amp;reserved=0" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
+    <hyperlink ref="B651" r:id="rId399" display="Newjoiner and resigner's expense" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
+    <hyperlink ref="B652" r:id="rId400" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
+    <hyperlink ref="B655" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
+    <hyperlink ref="B656" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
+    <hyperlink ref="B657" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
+    <hyperlink ref="B658" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
+    <hyperlink ref="B660" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
+    <hyperlink ref="B661" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
+    <hyperlink ref="B662" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
+    <hyperlink ref="B663" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
+    <hyperlink ref="B664" r:id="rId409" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
+    <hyperlink ref="B665" r:id="rId410" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
+    <hyperlink ref="B667" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
+    <hyperlink ref="B668" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
+    <hyperlink ref="B669" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
+    <hyperlink ref="B670" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
+    <hyperlink ref="B671" r:id="rId415" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
+    <hyperlink ref="B672" r:id="rId416" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
+    <hyperlink ref="B673" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
+    <hyperlink ref="B674" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
+    <hyperlink ref="B666" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId420"/>
@@ -52074,7 +52077,7 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Category!$A$2:$A$25</xm:f>
           </x14:formula1>
@@ -52087,7 +52090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -52236,7 +52239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -52322,7 +52325,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Commit Mar 16 v2
</commit_message>
<xml_diff>
--- a/KDB.xlsx
+++ b/KDB.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\DFS\JPHQ\AL\BUSUNITS\AL-Finance\Fin-FRA\JDE\02_AP\0356_KDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037EE1C2-0384-4911-A047-135D8955329E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664B3931-B14D-4D12-9873-24C86DFE65AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SOP" sheetId="4" r:id="rId1"/>
-    <sheet name="Master" sheetId="1" r:id="rId2"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="SOP" sheetId="4" r:id="rId2"/>
     <sheet name="Category" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Master!$A$1:$H$724</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$H$724</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4928,112 +4928,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="6.36328125" customWidth="1"/>
-    <col min="2" max="2" width="65.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="27" customFormat="1" ht="39" customHeight="1">
-      <c r="A1" s="24"/>
-      <c r="B1" s="25" t="s">
-        <v>325</v>
-      </c>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" customHeight="1">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="41" customHeight="1">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="87">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="72.5">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <customProperties>
-    <customPr name="_pios_id" r:id="rId3"/>
-  </customProperties>
-  <drawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H9998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="C716" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="11" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -53056,6 +52958,104 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="6.36328125" customWidth="1"/>
+    <col min="2" max="2" width="65.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="27" customFormat="1" ht="39" customHeight="1">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="C1" s="26"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" customHeight="1">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="41" customHeight="1">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="87">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72.5">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId3"/>
+  </customProperties>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B21"/>

</xml_diff>